<commit_message>
Add saving the output to csv, add automatic file download
</commit_message>
<xml_diff>
--- a/literature_search/LoS_incentives_revision_micro.xlsx
+++ b/literature_search/LoS_incentives_revision_micro.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jf41513/code/meta/incentives/literature_search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5715B273-C12F-474C-9B95-E7F268EF4286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7394F592-6AAB-414F-9E5E-6060BE6E863E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29400" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Studies" sheetId="13" r:id="rId1"/>
     <sheet name="Journals" sheetId="12" r:id="rId2"/>
-    <sheet name="2 AER" sheetId="1" r:id="rId3"/>
+    <sheet name="studies_py" sheetId="14" r:id="rId3"/>
+    <sheet name="2 AER" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="173">
   <si>
     <t>Number</t>
   </si>
@@ -2258,9 +2259,6 @@
   </si>
   <si>
     <t>Rank</t>
-  </si>
-  <si>
-    <t>Journals</t>
   </si>
   <si>
     <t>Score</t>
@@ -3191,7 +3189,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3216,40 +3214,40 @@
         <v>131</v>
       </c>
       <c r="B1" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="C1" s="51" t="s">
-        <v>173</v>
-      </c>
-      <c r="D1" s="49" t="s">
+      <c r="E1" s="49" t="s">
         <v>133</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="F1" s="50" t="s">
         <v>134</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="G1" s="50" t="s">
         <v>135</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="H1" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="I1" s="50" t="s">
         <v>137</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="J1" s="50" t="s">
         <v>138</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="K1" s="50" t="s">
         <v>139</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="L1" s="50" t="s">
         <v>140</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="M1" s="50" t="s">
         <v>141</v>
-      </c>
-      <c r="M1" s="50" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -3257,7 +3255,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C31" si="0">LEFT(B2,FIND(",", B2) - 1)</f>
@@ -3299,7 +3297,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="0"/>
@@ -3341,7 +3339,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -3383,7 +3381,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -3425,7 +3423,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -3467,7 +3465,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="46" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -3509,7 +3507,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -3551,7 +3549,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -3593,7 +3591,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -3635,7 +3633,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -3677,7 +3675,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -3719,7 +3717,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -3761,7 +3759,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="46" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -3803,7 +3801,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
@@ -3845,7 +3843,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -3887,7 +3885,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="46" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -3929,7 +3927,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="46" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -3971,7 +3969,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="46" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
@@ -4013,7 +4011,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
@@ -4055,7 +4053,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
@@ -4097,7 +4095,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="46" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
@@ -4139,7 +4137,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="46" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
@@ -4181,7 +4179,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
@@ -4223,7 +4221,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
@@ -4265,7 +4263,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
@@ -4307,7 +4305,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="46" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
@@ -4349,7 +4347,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
@@ -4391,7 +4389,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
@@ -4433,7 +4431,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="46" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
@@ -4475,7 +4473,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="46" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
@@ -4528,6 +4526,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA734DCB-1F42-A14A-A96C-EB8C68C09043}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>

</xml_diff>

<commit_message>
Search metadata is now saved upon search run end
</commit_message>
<xml_diff>
--- a/literature_search/LoS_incentives_revision_micro.xlsx
+++ b/literature_search/LoS_incentives_revision_micro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jf41513/code/meta/incentives/literature_search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDF8B9A-E854-B541-A73D-DBFF1C01B7C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34942E4A-2017-FF4C-ACC5-58835BCDA90E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29400" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2950,8 +2950,8 @@
   </sheetPr>
   <dimension ref="A1:H265"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A247" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F285" sqref="F285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Add identification for a number of the revision studies
</commit_message>
<xml_diff>
--- a/literature_search/LoS_incentives_revision_micro.xlsx
+++ b/literature_search/LoS_incentives_revision_micro.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jf41513/code/meta/incentives/literature_search/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petr/code/meta/incentives/literature_search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480831FE-1DF2-6A48-94F5-645F1C34D1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AE755D-7DF4-DB47-91C4-909FD64056DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Studies" sheetId="13" r:id="rId1"/>
-    <sheet name="Journals" sheetId="12" r:id="rId2"/>
-    <sheet name="Metadata" sheetId="15" r:id="rId3"/>
+    <sheet name="Metadata" sheetId="15" r:id="rId2"/>
+    <sheet name="Journals" sheetId="12" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="834">
   <si>
     <t>Journal</t>
   </si>
@@ -2504,13 +2504,49 @@
   </si>
   <si>
     <t>Quarterly Journal of Economics</t>
+  </si>
+  <si>
+    <t>Not found in the original search query, included in the new sample</t>
+  </si>
+  <si>
+    <t>Not found in the original search query, not included in the new sample</t>
+  </si>
+  <si>
+    <t>Mistake during the original selection</t>
+  </si>
+  <si>
+    <t>Done:</t>
+  </si>
+  <si>
+    <t>Misaligned query hit</t>
+  </si>
+  <si>
+    <t>No financial incentives</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Unmeasurable performance; New</t>
+  </si>
+  <si>
+    <t>A theoretical paper; New</t>
+  </si>
+  <si>
+    <t>Irrelevant to the topic</t>
+  </si>
+  <si>
+    <t>Irrelevant focus</t>
+  </si>
+  <si>
+    <t>No collectible data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2578,8 +2614,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2670,6 +2720,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -2689,11 +2751,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2726,16 +2789,20 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3025,8 +3092,8 @@
   </sheetPr>
   <dimension ref="A1:I265"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="C23" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3091,7 +3158,7 @@
         <v>24</v>
       </c>
       <c r="G2" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="9" t="s">
@@ -3118,9 +3185,11 @@
         <v>23</v>
       </c>
       <c r="G3" s="10">
-        <v>0</v>
-      </c>
-      <c r="H3" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>824</v>
+      </c>
       <c r="I3" s="9" t="s">
         <v>44</v>
       </c>
@@ -3145,9 +3214,11 @@
         <v>46</v>
       </c>
       <c r="G4" s="10">
-        <v>0</v>
-      </c>
-      <c r="H4" s="10"/>
+        <v>6</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>829</v>
+      </c>
       <c r="I4" s="9" t="s">
         <v>47</v>
       </c>
@@ -3172,7 +3243,7 @@
         <v>49</v>
       </c>
       <c r="G5" s="10">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>809</v>
@@ -3201,7 +3272,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="9" t="s">
@@ -3228,7 +3299,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="9" t="s">
@@ -3255,9 +3326,11 @@
         <v>6</v>
       </c>
       <c r="G8" s="10">
-        <v>0</v>
-      </c>
-      <c r="H8" s="10"/>
+        <v>4</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>809</v>
+      </c>
       <c r="I8" s="9" t="s">
         <v>56</v>
       </c>
@@ -3282,9 +3355,11 @@
         <v>9</v>
       </c>
       <c r="G9" s="10">
-        <v>0</v>
-      </c>
-      <c r="H9" s="10"/>
+        <v>4</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>809</v>
+      </c>
       <c r="I9" s="9" t="s">
         <v>58</v>
       </c>
@@ -3309,9 +3384,11 @@
         <v>19</v>
       </c>
       <c r="G10" s="10">
-        <v>0</v>
-      </c>
-      <c r="H10" s="10"/>
+        <v>4</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>826</v>
+      </c>
       <c r="I10" s="9" t="s">
         <v>59</v>
       </c>
@@ -3336,9 +3413,11 @@
         <v>4</v>
       </c>
       <c r="G11" s="10">
-        <v>0</v>
-      </c>
-      <c r="H11" s="10"/>
+        <v>4</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>827</v>
+      </c>
       <c r="I11" s="9" t="s">
         <v>61</v>
       </c>
@@ -3363,9 +3442,11 @@
         <v>7</v>
       </c>
       <c r="G12" s="10">
-        <v>0</v>
-      </c>
-      <c r="H12" s="10"/>
+        <v>4</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>827</v>
+      </c>
       <c r="I12" s="9" t="s">
         <v>63</v>
       </c>
@@ -3390,7 +3471,7 @@
         <v>10</v>
       </c>
       <c r="G13" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="9" t="s">
@@ -3417,9 +3498,11 @@
         <v>67</v>
       </c>
       <c r="G14" s="10">
-        <v>0</v>
-      </c>
-      <c r="H14" s="10"/>
+        <v>5</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>828</v>
+      </c>
       <c r="I14" s="9" t="s">
         <v>68</v>
       </c>
@@ -3444,7 +3527,7 @@
         <v>5</v>
       </c>
       <c r="G15" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="9" t="s">
@@ -3471,7 +3554,7 @@
         <v>8</v>
       </c>
       <c r="G16" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="9" t="s">
@@ -3498,9 +3581,11 @@
         <v>13</v>
       </c>
       <c r="G17" s="10">
-        <v>0</v>
-      </c>
-      <c r="H17" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>824</v>
+      </c>
       <c r="I17" s="9" t="s">
         <v>74</v>
       </c>
@@ -3525,9 +3610,11 @@
         <v>15</v>
       </c>
       <c r="G18" s="10">
-        <v>0</v>
-      </c>
-      <c r="H18" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>824</v>
+      </c>
       <c r="I18" s="9" t="s">
         <v>76</v>
       </c>
@@ -3552,9 +3639,11 @@
         <v>17</v>
       </c>
       <c r="G19" s="10">
-        <v>0</v>
-      </c>
-      <c r="H19" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>824</v>
+      </c>
       <c r="I19" s="9" t="s">
         <v>78</v>
       </c>
@@ -3579,9 +3668,11 @@
         <v>81</v>
       </c>
       <c r="G20" s="10">
-        <v>0</v>
-      </c>
-      <c r="H20" s="10"/>
+        <v>6</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>830</v>
+      </c>
       <c r="I20" s="9" t="s">
         <v>82</v>
       </c>
@@ -3606,9 +3697,11 @@
         <v>14</v>
       </c>
       <c r="G21" s="10">
-        <v>0</v>
-      </c>
-      <c r="H21" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>824</v>
+      </c>
       <c r="I21" s="9" t="s">
         <v>84</v>
       </c>
@@ -3633,9 +3726,11 @@
         <v>19</v>
       </c>
       <c r="G22" s="10">
-        <v>0</v>
-      </c>
-      <c r="H22" s="10"/>
+        <v>4</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>826</v>
+      </c>
       <c r="I22" s="9" t="s">
         <v>86</v>
       </c>
@@ -3660,9 +3755,11 @@
         <v>88</v>
       </c>
       <c r="G23" s="10">
-        <v>0</v>
-      </c>
-      <c r="H23" s="10"/>
+        <v>6</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>826</v>
+      </c>
       <c r="I23" s="9" t="s">
         <v>89</v>
       </c>
@@ -3687,7 +3784,7 @@
         <v>91</v>
       </c>
       <c r="G24" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="9" t="s">
@@ -3714,9 +3811,11 @@
         <v>94</v>
       </c>
       <c r="G25" s="10">
-        <v>0</v>
-      </c>
-      <c r="H25" s="10"/>
+        <v>6</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>831</v>
+      </c>
       <c r="I25" s="9" t="s">
         <v>95</v>
       </c>
@@ -3741,9 +3840,11 @@
         <v>21</v>
       </c>
       <c r="G26" s="10">
-        <v>0</v>
-      </c>
-      <c r="H26" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>824</v>
+      </c>
       <c r="I26" s="9" t="s">
         <v>97</v>
       </c>
@@ -3768,9 +3869,11 @@
         <v>12</v>
       </c>
       <c r="G27" s="10">
-        <v>0</v>
-      </c>
-      <c r="H27" s="10"/>
+        <v>6</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>832</v>
+      </c>
       <c r="I27" s="9" t="s">
         <v>99</v>
       </c>
@@ -3795,9 +3898,11 @@
         <v>18</v>
       </c>
       <c r="G28" s="10">
-        <v>0</v>
-      </c>
-      <c r="H28" s="10"/>
+        <v>4</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>833</v>
+      </c>
       <c r="I28" s="9" t="s">
         <v>101</v>
       </c>
@@ -3822,9 +3927,11 @@
         <v>16</v>
       </c>
       <c r="G29" s="10">
-        <v>0</v>
-      </c>
-      <c r="H29" s="10"/>
+        <v>4</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>833</v>
+      </c>
       <c r="I29" s="9" t="s">
         <v>103</v>
       </c>
@@ -3849,9 +3956,11 @@
         <v>11</v>
       </c>
       <c r="G30" s="10">
-        <v>0</v>
-      </c>
-      <c r="H30" s="10"/>
+        <v>6</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>809</v>
+      </c>
       <c r="I30" s="9" t="s">
         <v>105</v>
       </c>
@@ -3876,9 +3985,11 @@
         <v>20</v>
       </c>
       <c r="G31" s="10">
-        <v>0</v>
-      </c>
-      <c r="H31" s="10"/>
+        <v>4</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>809</v>
+      </c>
       <c r="I31" s="9" t="s">
         <v>107</v>
       </c>
@@ -3903,9 +4014,11 @@
         <v>109</v>
       </c>
       <c r="G32" s="10">
-        <v>0</v>
-      </c>
-      <c r="H32" s="10"/>
+        <v>6</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>832</v>
+      </c>
       <c r="I32" s="9" t="s">
         <v>110</v>
       </c>
@@ -3930,7 +4043,7 @@
         <v>112</v>
       </c>
       <c r="G33" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H33" s="10"/>
       <c r="I33" s="9" t="s">
@@ -3957,9 +4070,11 @@
         <v>116</v>
       </c>
       <c r="G34" s="10">
-        <v>0</v>
-      </c>
-      <c r="H34" s="10"/>
+        <v>6</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>832</v>
+      </c>
       <c r="I34" s="9" t="s">
         <v>117</v>
       </c>
@@ -10207,13 +10322,221 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81CCFCCB-8546-F94C-8848-7B181B7F20C3}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>804</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>802</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="17">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <f>COUNTIF(Studies!G:G, E11)</f>
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="D12" s="32"/>
+      <c r="E12" s="14">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <f>COUNTIF(Studies!G:G, E12)</f>
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="D13" s="32"/>
+      <c r="E13" s="24">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <f>COUNTIF(Studies!G:G, E13)</f>
+        <v>6</v>
+      </c>
+      <c r="G13" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="D14" s="32"/>
+      <c r="E14" s="25">
+        <v>4</v>
+      </c>
+      <c r="F14">
+        <f>COUNTIF(Studies!G:G, E14)</f>
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="D15" s="32"/>
+      <c r="E15" s="30">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <f>COUNTIF(Studies!G:G, E15)</f>
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="D16" s="32"/>
+      <c r="E16" s="29">
+        <v>6</v>
+      </c>
+      <c r="F16">
+        <f>COUNTIF(Studies!G:G, E16)</f>
+        <v>9</v>
+      </c>
+      <c r="G16" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7">
+      <c r="D17" s="15" t="s">
+        <v>798</v>
+      </c>
+      <c r="E17" s="18">
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <f>COUNTIF(Studies!G:G, E17)</f>
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7">
+      <c r="D18" s="28" t="s">
+        <v>807</v>
+      </c>
+      <c r="E18" s="19">
+        <v>8</v>
+      </c>
+      <c r="F18">
+        <f>COUNTIF(Studies!G:G, E18)</f>
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7">
+      <c r="D19" s="28"/>
+      <c r="E19" s="20">
+        <v>9</v>
+      </c>
+      <c r="F19">
+        <f>COUNTIF(Studies!G:G, E19)</f>
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7">
+      <c r="D20" s="16" t="s">
+        <v>806</v>
+      </c>
+      <c r="E20" s="13">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f>COUNTIF(Studies!G:G, E20)</f>
+        <v>231</v>
+      </c>
+      <c r="G20" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="22" spans="4:7">
+      <c r="D22" t="s">
+        <v>825</v>
+      </c>
+      <c r="E22" s="31">
+        <f>SUM(F11:F19)/(F20+SUM(F11:F19))</f>
+        <v>0.125</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D11:D16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AFAFB47-306A-E946-B821-EFD954047C06}">
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:M89"/>
   <sheetViews>
-    <sheetView zoomScale="108" workbookViewId="0">
+    <sheetView zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -11213,178 +11536,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81CCFCCB-8546-F94C-8848-7B181B7F20C3}">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:G18"/>
-  <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="7" max="7" width="14.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>804</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>802</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="17">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <f>COUNTIF(Studies!G:G, E11)</f>
-        <v>0</v>
-      </c>
-      <c r="G11" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="D12" s="28"/>
-      <c r="E12" s="14">
-        <v>2</v>
-      </c>
-      <c r="F12">
-        <f>COUNTIF(Studies!G:G, E12)</f>
-        <v>0</v>
-      </c>
-      <c r="G12" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="D13" s="28"/>
-      <c r="E13" s="24">
-        <v>3</v>
-      </c>
-      <c r="F13">
-        <f>COUNTIF(Studies!G:G, E13)</f>
-        <v>0</v>
-      </c>
-      <c r="G13" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="D14" s="28"/>
-      <c r="E14" s="25">
-        <v>4</v>
-      </c>
-      <c r="F14">
-        <f>COUNTIF(Studies!G:G, E14)</f>
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="D15" s="15" t="s">
-        <v>798</v>
-      </c>
-      <c r="E15" s="18">
-        <v>5</v>
-      </c>
-      <c r="F15">
-        <f>COUNTIF(Studies!G:G, E15)</f>
-        <v>0</v>
-      </c>
-      <c r="G15" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="D16" s="29" t="s">
-        <v>807</v>
-      </c>
-      <c r="E16" s="19">
-        <v>6</v>
-      </c>
-      <c r="F16">
-        <f>COUNTIF(Studies!G:G, E16)</f>
-        <v>0</v>
-      </c>
-      <c r="G16" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="17" spans="4:7">
-      <c r="D17" s="29"/>
-      <c r="E17" s="20">
-        <v>7</v>
-      </c>
-      <c r="F17">
-        <f>COUNTIF(Studies!G:G, E17)</f>
-        <v>0</v>
-      </c>
-      <c r="G17" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="18" spans="4:7">
-      <c r="D18" s="16" t="s">
-        <v>806</v>
-      </c>
-      <c r="E18" s="13">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <f>COUNTIF(Studies!G:G, E18)</f>
-        <v>263</v>
-      </c>
-      <c r="G18" t="s">
-        <v>805</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="D16:D17"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Revise more incentives re-search papers
</commit_message>
<xml_diff>
--- a/literature_search/LoS_incentives_revision_micro.xlsx
+++ b/literature_search/LoS_incentives_revision_micro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petr/code/meta/incentives/literature_search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C36500E-9513-3140-A65D-4A449B21C7C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA938AD-370C-B74C-882E-AC7B4406059C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="55120" yWindow="0" windowWidth="25480" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52140" yWindow="0" windowWidth="28460" windowHeight="28800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Studies" sheetId="13" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="854">
   <si>
     <t>Journal</t>
   </si>
@@ -2582,6 +2582,24 @@
   </si>
   <si>
     <t>Total papers:</t>
+  </si>
+  <si>
+    <t>Invalid search</t>
+  </si>
+  <si>
+    <t>Invalid search item, such as duplicates, or from another journal</t>
+  </si>
+  <si>
+    <t>Incorrect paper</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Meta-analysis with a different focus</t>
+  </si>
+  <si>
+    <t>Meta-analysis</t>
   </si>
 </sst>
 </file>
@@ -2678,7 +2696,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2781,6 +2799,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -2805,7 +2835,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2836,9 +2866,6 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
@@ -2849,6 +2876,13 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3143,8 +3177,8 @@
   </sheetPr>
   <dimension ref="A1:I265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
-      <selection activeCell="H85" sqref="H85"/>
+    <sheetView topLeftCell="B103" zoomScale="159" zoomScaleNormal="131" workbookViewId="0">
+      <selection activeCell="F124" sqref="F124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3155,8 +3189,8 @@
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.5" customWidth="1"/>
     <col min="6" max="6" width="33" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" style="34" customWidth="1"/>
-    <col min="8" max="8" width="27.83203125" style="34" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="33" customWidth="1"/>
+    <col min="8" max="8" width="27.83203125" style="33" customWidth="1"/>
     <col min="9" max="9" width="190.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3208,10 +3242,10 @@
       <c r="F2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="32">
+      <c r="G2" s="31">
         <v>1</v>
       </c>
-      <c r="H2" s="32"/>
+      <c r="H2" s="31"/>
       <c r="I2" s="9" t="s">
         <v>42</v>
       </c>
@@ -3235,10 +3269,10 @@
       <c r="F3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="32">
+      <c r="G3" s="31">
         <v>3</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="31" t="s">
         <v>824</v>
       </c>
       <c r="I3" s="9" t="s">
@@ -3264,10 +3298,10 @@
       <c r="F4" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="32">
+      <c r="G4" s="31">
         <v>6</v>
       </c>
-      <c r="H4" s="32" t="s">
+      <c r="H4" s="31" t="s">
         <v>829</v>
       </c>
       <c r="I4" s="9" t="s">
@@ -3293,10 +3327,10 @@
       <c r="F5" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="32">
+      <c r="G5" s="31">
         <v>6</v>
       </c>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="31" t="s">
         <v>809</v>
       </c>
       <c r="I5" s="9" t="s">
@@ -3322,10 +3356,10 @@
       <c r="F6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="32">
+      <c r="G6" s="31">
         <v>1</v>
       </c>
-      <c r="H6" s="32"/>
+      <c r="H6" s="31"/>
       <c r="I6" s="9" t="s">
         <v>52</v>
       </c>
@@ -3349,10 +3383,10 @@
       <c r="F7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="32">
+      <c r="G7" s="31">
         <v>4</v>
       </c>
-      <c r="H7" s="32"/>
+      <c r="H7" s="31"/>
       <c r="I7" s="9" t="s">
         <v>54</v>
       </c>
@@ -3376,10 +3410,10 @@
       <c r="F8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="31">
         <v>4</v>
       </c>
-      <c r="H8" s="32" t="s">
+      <c r="H8" s="31" t="s">
         <v>809</v>
       </c>
       <c r="I8" s="9" t="s">
@@ -3405,10 +3439,10 @@
       <c r="F9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="32">
+      <c r="G9" s="31">
         <v>4</v>
       </c>
-      <c r="H9" s="32" t="s">
+      <c r="H9" s="31" t="s">
         <v>809</v>
       </c>
       <c r="I9" s="9" t="s">
@@ -3434,10 +3468,10 @@
       <c r="F10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="32">
+      <c r="G10" s="31">
         <v>4</v>
       </c>
-      <c r="H10" s="32" t="s">
+      <c r="H10" s="31" t="s">
         <v>826</v>
       </c>
       <c r="I10" s="9" t="s">
@@ -3463,10 +3497,10 @@
       <c r="F11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="32">
+      <c r="G11" s="31">
         <v>4</v>
       </c>
-      <c r="H11" s="32" t="s">
+      <c r="H11" s="31" t="s">
         <v>827</v>
       </c>
       <c r="I11" s="9" t="s">
@@ -3492,10 +3526,10 @@
       <c r="F12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="32">
+      <c r="G12" s="31">
         <v>4</v>
       </c>
-      <c r="H12" s="32" t="s">
+      <c r="H12" s="31" t="s">
         <v>827</v>
       </c>
       <c r="I12" s="9" t="s">
@@ -3521,10 +3555,10 @@
       <c r="F13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="32">
+      <c r="G13" s="31">
         <v>1</v>
       </c>
-      <c r="H13" s="32"/>
+      <c r="H13" s="31"/>
       <c r="I13" s="9" t="s">
         <v>65</v>
       </c>
@@ -3548,10 +3582,10 @@
       <c r="F14" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G14" s="32">
+      <c r="G14" s="31">
         <v>5</v>
       </c>
-      <c r="H14" s="32" t="s">
+      <c r="H14" s="31" t="s">
         <v>828</v>
       </c>
       <c r="I14" s="9" t="s">
@@ -3577,10 +3611,10 @@
       <c r="F15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G15" s="32">
+      <c r="G15" s="31">
         <v>1</v>
       </c>
-      <c r="H15" s="32"/>
+      <c r="H15" s="31"/>
       <c r="I15" s="9" t="s">
         <v>70</v>
       </c>
@@ -3604,10 +3638,10 @@
       <c r="F16" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="32">
+      <c r="G16" s="31">
         <v>1</v>
       </c>
-      <c r="H16" s="32"/>
+      <c r="H16" s="31"/>
       <c r="I16" s="9" t="s">
         <v>72</v>
       </c>
@@ -3631,10 +3665,10 @@
       <c r="F17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="32">
+      <c r="G17" s="31">
         <v>3</v>
       </c>
-      <c r="H17" s="32" t="s">
+      <c r="H17" s="31" t="s">
         <v>824</v>
       </c>
       <c r="I17" s="9" t="s">
@@ -3660,10 +3694,10 @@
       <c r="F18" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="32">
+      <c r="G18" s="31">
         <v>3</v>
       </c>
-      <c r="H18" s="32" t="s">
+      <c r="H18" s="31" t="s">
         <v>824</v>
       </c>
       <c r="I18" s="9" t="s">
@@ -3689,10 +3723,10 @@
       <c r="F19" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="32">
+      <c r="G19" s="31">
         <v>3</v>
       </c>
-      <c r="H19" s="32" t="s">
+      <c r="H19" s="31" t="s">
         <v>824</v>
       </c>
       <c r="I19" s="9" t="s">
@@ -3718,10 +3752,10 @@
       <c r="F20" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G20" s="32">
+      <c r="G20" s="31">
         <v>6</v>
       </c>
-      <c r="H20" s="32" t="s">
+      <c r="H20" s="31" t="s">
         <v>830</v>
       </c>
       <c r="I20" s="9" t="s">
@@ -3747,10 +3781,10 @@
       <c r="F21" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="32">
+      <c r="G21" s="31">
         <v>3</v>
       </c>
-      <c r="H21" s="32" t="s">
+      <c r="H21" s="31" t="s">
         <v>824</v>
       </c>
       <c r="I21" s="9" t="s">
@@ -3776,10 +3810,10 @@
       <c r="F22" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="32">
+      <c r="G22" s="31">
         <v>4</v>
       </c>
-      <c r="H22" s="32" t="s">
+      <c r="H22" s="31" t="s">
         <v>826</v>
       </c>
       <c r="I22" s="9" t="s">
@@ -3805,10 +3839,10 @@
       <c r="F23" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G23" s="32">
+      <c r="G23" s="31">
         <v>6</v>
       </c>
-      <c r="H23" s="32" t="s">
+      <c r="H23" s="31" t="s">
         <v>826</v>
       </c>
       <c r="I23" s="9" t="s">
@@ -3834,10 +3868,10 @@
       <c r="F24" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="G24" s="32">
+      <c r="G24" s="31">
         <v>5</v>
       </c>
-      <c r="H24" s="32"/>
+      <c r="H24" s="31"/>
       <c r="I24" s="9" t="s">
         <v>92</v>
       </c>
@@ -3861,10 +3895,10 @@
       <c r="F25" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="G25" s="32">
+      <c r="G25" s="31">
         <v>6</v>
       </c>
-      <c r="H25" s="32" t="s">
+      <c r="H25" s="31" t="s">
         <v>831</v>
       </c>
       <c r="I25" s="9" t="s">
@@ -3890,10 +3924,10 @@
       <c r="F26" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G26" s="32">
+      <c r="G26" s="31">
         <v>3</v>
       </c>
-      <c r="H26" s="32" t="s">
+      <c r="H26" s="31" t="s">
         <v>824</v>
       </c>
       <c r="I26" s="9" t="s">
@@ -3919,10 +3953,10 @@
       <c r="F27" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="32">
+      <c r="G27" s="31">
         <v>6</v>
       </c>
-      <c r="H27" s="32" t="s">
+      <c r="H27" s="31" t="s">
         <v>832</v>
       </c>
       <c r="I27" s="9" t="s">
@@ -3948,10 +3982,10 @@
       <c r="F28" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G28" s="32">
+      <c r="G28" s="31">
         <v>4</v>
       </c>
-      <c r="H28" s="32" t="s">
+      <c r="H28" s="31" t="s">
         <v>833</v>
       </c>
       <c r="I28" s="9" t="s">
@@ -3977,10 +4011,10 @@
       <c r="F29" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G29" s="32">
+      <c r="G29" s="31">
         <v>4</v>
       </c>
-      <c r="H29" s="32" t="s">
+      <c r="H29" s="31" t="s">
         <v>833</v>
       </c>
       <c r="I29" s="9" t="s">
@@ -4006,10 +4040,10 @@
       <c r="F30" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G30" s="32">
+      <c r="G30" s="31">
         <v>6</v>
       </c>
-      <c r="H30" s="32" t="s">
+      <c r="H30" s="31" t="s">
         <v>809</v>
       </c>
       <c r="I30" s="9" t="s">
@@ -4035,10 +4069,10 @@
       <c r="F31" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G31" s="32">
+      <c r="G31" s="31">
         <v>4</v>
       </c>
-      <c r="H31" s="32" t="s">
+      <c r="H31" s="31" t="s">
         <v>809</v>
       </c>
       <c r="I31" s="9" t="s">
@@ -4064,10 +4098,10 @@
       <c r="F32" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="G32" s="32">
+      <c r="G32" s="31">
         <v>6</v>
       </c>
-      <c r="H32" s="32" t="s">
+      <c r="H32" s="31" t="s">
         <v>832</v>
       </c>
       <c r="I32" s="9" t="s">
@@ -4093,10 +4127,10 @@
       <c r="F33" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="G33" s="32">
+      <c r="G33" s="31">
         <v>5</v>
       </c>
-      <c r="H33" s="32"/>
+      <c r="H33" s="31"/>
       <c r="I33" s="9" t="s">
         <v>113</v>
       </c>
@@ -4120,10 +4154,10 @@
       <c r="F34" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G34" s="32">
+      <c r="G34" s="31">
         <v>6</v>
       </c>
-      <c r="H34" s="32" t="s">
+      <c r="H34" s="31" t="s">
         <v>832</v>
       </c>
       <c r="I34" s="9" t="s">
@@ -4149,10 +4183,10 @@
       <c r="F35" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="G35" s="32">
+      <c r="G35" s="31">
         <v>6</v>
       </c>
-      <c r="H35" s="32" t="s">
+      <c r="H35" s="31" t="s">
         <v>832</v>
       </c>
       <c r="I35" s="9" t="s">
@@ -4178,10 +4212,10 @@
       <c r="F36" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="G36" s="32">
+      <c r="G36" s="31">
         <v>4</v>
       </c>
-      <c r="H36" s="32" t="s">
+      <c r="H36" s="31" t="s">
         <v>827</v>
       </c>
       <c r="I36" s="9" t="s">
@@ -4207,10 +4241,10 @@
       <c r="F37" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="G37" s="32">
+      <c r="G37" s="31">
         <v>4</v>
       </c>
-      <c r="H37" s="32" t="s">
+      <c r="H37" s="31" t="s">
         <v>838</v>
       </c>
       <c r="I37" s="9" t="s">
@@ -4236,10 +4270,10 @@
       <c r="F38" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G38" s="32">
+      <c r="G38" s="31">
         <v>4</v>
       </c>
-      <c r="H38" s="32" t="s">
+      <c r="H38" s="31" t="s">
         <v>832</v>
       </c>
       <c r="I38" s="9" t="s">
@@ -4265,10 +4299,10 @@
       <c r="F39" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="G39" s="32">
+      <c r="G39" s="31">
         <v>6</v>
       </c>
-      <c r="H39" s="32" t="s">
+      <c r="H39" s="31" t="s">
         <v>839</v>
       </c>
       <c r="I39" s="9" t="s">
@@ -4294,10 +4328,10 @@
       <c r="F40" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="G40" s="32">
+      <c r="G40" s="31">
         <v>3</v>
       </c>
-      <c r="H40" s="32" t="s">
+      <c r="H40" s="31" t="s">
         <v>824</v>
       </c>
       <c r="I40" s="9" t="s">
@@ -4323,10 +4357,10 @@
       <c r="F41" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="G41" s="32">
+      <c r="G41" s="31">
         <v>3</v>
       </c>
-      <c r="H41" s="32" t="s">
+      <c r="H41" s="31" t="s">
         <v>824</v>
       </c>
       <c r="I41" s="9" t="s">
@@ -4352,10 +4386,10 @@
       <c r="F42" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="G42" s="32">
+      <c r="G42" s="31">
         <v>4</v>
       </c>
-      <c r="H42" s="32" t="s">
+      <c r="H42" s="31" t="s">
         <v>832</v>
       </c>
       <c r="I42" s="9" t="s">
@@ -4381,10 +4415,10 @@
       <c r="F43" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="G43" s="32">
+      <c r="G43" s="31">
         <v>5</v>
       </c>
-      <c r="H43" s="32" t="s">
+      <c r="H43" s="31" t="s">
         <v>828</v>
       </c>
       <c r="I43" s="9" t="s">
@@ -4410,10 +4444,10 @@
       <c r="F44" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="G44" s="32">
+      <c r="G44" s="31">
         <v>6</v>
       </c>
-      <c r="H44" s="32" t="s">
+      <c r="H44" s="31" t="s">
         <v>840</v>
       </c>
       <c r="I44" s="9" t="s">
@@ -4439,10 +4473,10 @@
       <c r="F45" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G45" s="32">
+      <c r="G45" s="31">
         <v>6</v>
       </c>
-      <c r="H45" s="32" t="s">
+      <c r="H45" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I45" s="9" t="s">
@@ -4468,10 +4502,10 @@
       <c r="F46" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="G46" s="32">
+      <c r="G46" s="31">
         <v>6</v>
       </c>
-      <c r="H46" s="32" t="s">
+      <c r="H46" s="31" t="s">
         <v>842</v>
       </c>
       <c r="I46" s="9" t="s">
@@ -4497,10 +4531,10 @@
       <c r="F47" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="G47" s="32">
+      <c r="G47" s="31">
         <v>6</v>
       </c>
-      <c r="H47" s="32" t="s">
+      <c r="H47" s="31" t="s">
         <v>832</v>
       </c>
       <c r="I47" s="9" t="s">
@@ -4526,10 +4560,10 @@
       <c r="F48" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="G48" s="32">
+      <c r="G48" s="31">
         <v>4</v>
       </c>
-      <c r="H48" s="32" t="s">
+      <c r="H48" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I48" s="9" t="s">
@@ -4555,10 +4589,10 @@
       <c r="F49" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="G49" s="32">
+      <c r="G49" s="31">
         <v>4</v>
       </c>
-      <c r="H49" s="32" t="s">
+      <c r="H49" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I49" s="9" t="s">
@@ -4584,10 +4618,10 @@
       <c r="F50" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="G50" s="32">
+      <c r="G50" s="31">
         <v>5</v>
       </c>
-      <c r="H50" s="32" t="s">
+      <c r="H50" s="31" t="s">
         <v>828</v>
       </c>
       <c r="I50" s="9" t="s">
@@ -4613,10 +4647,10 @@
       <c r="F51" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="G51" s="32">
-        <v>4</v>
-      </c>
-      <c r="H51" s="32" t="s">
+      <c r="G51" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H51" s="31" t="s">
         <v>837</v>
       </c>
       <c r="I51" s="9" t="s">
@@ -4642,10 +4676,10 @@
       <c r="F52" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="G52" s="32">
+      <c r="G52" s="31">
         <v>6</v>
       </c>
-      <c r="H52" s="32" t="s">
+      <c r="H52" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I52" s="9" t="s">
@@ -4671,10 +4705,10 @@
       <c r="F53" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="G53" s="32">
+      <c r="G53" s="31">
         <v>6</v>
       </c>
-      <c r="H53" s="32" t="s">
+      <c r="H53" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I53" s="9" t="s">
@@ -4700,10 +4734,10 @@
       <c r="F54" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="G54" s="32">
+      <c r="G54" s="31">
         <v>6</v>
       </c>
-      <c r="H54" s="32" t="s">
+      <c r="H54" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I54" s="9" t="s">
@@ -4729,10 +4763,10 @@
       <c r="F55" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="G55" s="32">
+      <c r="G55" s="31">
         <v>6</v>
       </c>
-      <c r="H55" s="32" t="s">
+      <c r="H55" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I55" s="9" t="s">
@@ -4758,10 +4792,10 @@
       <c r="F56" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="G56" s="32">
+      <c r="G56" s="31">
         <v>4</v>
       </c>
-      <c r="H56" s="32" t="s">
+      <c r="H56" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I56" s="9" t="s">
@@ -4787,10 +4821,10 @@
       <c r="F57" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G57" s="32">
+      <c r="G57" s="31">
         <v>6</v>
       </c>
-      <c r="H57" s="32" t="s">
+      <c r="H57" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I57" s="9" t="s">
@@ -4816,10 +4850,10 @@
       <c r="F58" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="G58" s="32">
+      <c r="G58" s="31">
         <v>4</v>
       </c>
-      <c r="H58" s="32" t="s">
+      <c r="H58" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I58" s="9" t="s">
@@ -4845,10 +4879,10 @@
       <c r="F59" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="G59" s="32">
+      <c r="G59" s="31">
         <v>4</v>
       </c>
-      <c r="H59" s="32" t="s">
+      <c r="H59" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I59" s="9" t="s">
@@ -4874,10 +4908,10 @@
       <c r="F60" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="G60" s="32">
+      <c r="G60" s="31">
         <v>4</v>
       </c>
-      <c r="H60" s="32" t="s">
+      <c r="H60" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I60" s="9" t="s">
@@ -4903,10 +4937,10 @@
       <c r="F61" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="G61" s="32">
+      <c r="G61" s="31">
         <v>4</v>
       </c>
-      <c r="H61" s="32" t="s">
+      <c r="H61" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I61" s="9" t="s">
@@ -4932,10 +4966,10 @@
       <c r="F62" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="G62" s="32">
+      <c r="G62" s="31">
         <v>4</v>
       </c>
-      <c r="H62" s="32" t="s">
+      <c r="H62" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I62" s="9" t="s">
@@ -4961,10 +4995,10 @@
       <c r="F63" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="G63" s="32">
+      <c r="G63" s="31">
         <v>4</v>
       </c>
-      <c r="H63" s="32" t="s">
+      <c r="H63" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I63" s="9" t="s">
@@ -4990,10 +5024,10 @@
       <c r="F64" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="G64" s="32">
+      <c r="G64" s="31">
         <v>4</v>
       </c>
-      <c r="H64" s="32" t="s">
+      <c r="H64" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I64" s="9" t="s">
@@ -5019,10 +5053,10 @@
       <c r="F65" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="G65" s="32">
+      <c r="G65" s="31">
         <v>4</v>
       </c>
-      <c r="H65" s="32" t="s">
+      <c r="H65" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I65" s="9" t="s">
@@ -5048,10 +5082,10 @@
       <c r="F66" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="G66" s="32">
+      <c r="G66" s="31">
         <v>4</v>
       </c>
-      <c r="H66" s="32" t="s">
+      <c r="H66" s="31" t="s">
         <v>831</v>
       </c>
       <c r="I66" s="9" t="s">
@@ -5077,10 +5111,10 @@
       <c r="F67" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="G67" s="32">
+      <c r="G67" s="31">
         <v>6</v>
       </c>
-      <c r="H67" s="32" t="s">
+      <c r="H67" s="31" t="s">
         <v>843</v>
       </c>
       <c r="I67" s="9" t="s">
@@ -5106,10 +5140,10 @@
       <c r="F68" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="G68" s="32">
+      <c r="G68" s="31">
         <v>6</v>
       </c>
-      <c r="H68" s="32" t="s">
+      <c r="H68" s="31" t="s">
         <v>831</v>
       </c>
       <c r="I68" s="9" t="s">
@@ -5135,10 +5169,10 @@
       <c r="F69" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="G69" s="32">
+      <c r="G69" s="31">
         <v>6</v>
       </c>
-      <c r="H69" s="32" t="s">
+      <c r="H69" s="31" t="s">
         <v>844</v>
       </c>
       <c r="I69" s="9" t="s">
@@ -5164,10 +5198,10 @@
       <c r="F70" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="G70" s="32">
+      <c r="G70" s="31">
         <v>4</v>
       </c>
-      <c r="H70" s="32" t="s">
+      <c r="H70" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I70" s="9" t="s">
@@ -5193,10 +5227,10 @@
       <c r="F71" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="G71" s="32">
+      <c r="G71" s="31">
         <v>4</v>
       </c>
-      <c r="H71" s="32" t="s">
+      <c r="H71" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I71" s="9" t="s">
@@ -5222,10 +5256,10 @@
       <c r="F72" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="G72" s="32">
+      <c r="G72" s="31">
         <v>4</v>
       </c>
-      <c r="H72" s="32" t="s">
+      <c r="H72" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I72" s="9" t="s">
@@ -5251,10 +5285,10 @@
       <c r="F73" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="G73" s="32">
+      <c r="G73" s="31">
         <v>4</v>
       </c>
-      <c r="H73" s="32" t="s">
+      <c r="H73" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I73" s="9" t="s">
@@ -5280,10 +5314,10 @@
       <c r="F74" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="G74" s="32">
+      <c r="G74" s="31">
         <v>4</v>
       </c>
-      <c r="H74" s="32" t="s">
+      <c r="H74" s="31" t="s">
         <v>832</v>
       </c>
       <c r="I74" s="9" t="s">
@@ -5309,10 +5343,10 @@
       <c r="F75" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="G75" s="32">
+      <c r="G75" s="31">
         <v>4</v>
       </c>
-      <c r="H75" s="32" t="s">
+      <c r="H75" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I75" s="9" t="s">
@@ -5338,10 +5372,10 @@
       <c r="F76" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="G76" s="32">
+      <c r="G76" s="31">
         <v>4</v>
       </c>
-      <c r="H76" s="32" t="s">
+      <c r="H76" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I76" s="9" t="s">
@@ -5367,10 +5401,10 @@
       <c r="F77" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="G77" s="32">
+      <c r="G77" s="31">
         <v>4</v>
       </c>
-      <c r="H77" s="32" t="s">
+      <c r="H77" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I77" s="9" t="s">
@@ -5396,10 +5430,10 @@
       <c r="F78" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="G78" s="32">
+      <c r="G78" s="31">
         <v>4</v>
       </c>
-      <c r="H78" s="32" t="s">
+      <c r="H78" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I78" s="9" t="s">
@@ -5425,10 +5459,10 @@
       <c r="F79" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="G79" s="32">
+      <c r="G79" s="31">
         <v>5</v>
       </c>
-      <c r="H79" s="32" t="s">
+      <c r="H79" s="31" t="s">
         <v>828</v>
       </c>
       <c r="I79" s="9" t="s">
@@ -5454,10 +5488,10 @@
       <c r="F80" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="G80" s="32">
+      <c r="G80" s="31">
         <v>3</v>
       </c>
-      <c r="H80" s="32" t="s">
+      <c r="H80" s="31" t="s">
         <v>824</v>
       </c>
       <c r="I80" s="9" t="s">
@@ -5483,10 +5517,10 @@
       <c r="F81" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="G81" s="32">
+      <c r="G81" s="31">
         <v>4</v>
       </c>
-      <c r="H81" s="32" t="s">
+      <c r="H81" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I81" s="9" t="s">
@@ -5512,10 +5546,10 @@
       <c r="F82" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="G82" s="32">
+      <c r="G82" s="31">
         <v>5</v>
       </c>
-      <c r="H82" s="32" t="s">
+      <c r="H82" s="31" t="s">
         <v>828</v>
       </c>
       <c r="I82" s="9" t="s">
@@ -5541,10 +5575,10 @@
       <c r="F83" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="G83" s="32">
+      <c r="G83" s="31">
         <v>4</v>
       </c>
-      <c r="H83" s="32" t="s">
+      <c r="H83" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I83" s="9" t="s">
@@ -5570,10 +5604,10 @@
       <c r="F84" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="G84" s="32">
+      <c r="G84" s="31">
         <v>6</v>
       </c>
-      <c r="H84" s="32" t="s">
+      <c r="H84" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I84" s="9" t="s">
@@ -5599,10 +5633,10 @@
       <c r="F85" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="G85" s="32">
+      <c r="G85" s="31">
         <v>4</v>
       </c>
-      <c r="H85" s="32" t="s">
+      <c r="H85" s="31" t="s">
         <v>841</v>
       </c>
       <c r="I85" s="9" t="s">
@@ -5628,10 +5662,12 @@
       <c r="F86" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="G86" s="32">
-        <v>0</v>
-      </c>
-      <c r="H86" s="32"/>
+      <c r="G86" s="31">
+        <v>4</v>
+      </c>
+      <c r="H86" s="31" t="s">
+        <v>841</v>
+      </c>
       <c r="I86" s="9" t="s">
         <v>276</v>
       </c>
@@ -5655,10 +5691,12 @@
       <c r="F87" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="G87" s="32">
-        <v>0</v>
-      </c>
-      <c r="H87" s="32"/>
+      <c r="G87" s="31">
+        <v>4</v>
+      </c>
+      <c r="H87" s="31" t="s">
+        <v>841</v>
+      </c>
       <c r="I87" s="9" t="s">
         <v>279</v>
       </c>
@@ -5682,10 +5720,12 @@
       <c r="F88" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="G88" s="32">
-        <v>0</v>
-      </c>
-      <c r="H88" s="32"/>
+      <c r="G88" s="31">
+        <v>4</v>
+      </c>
+      <c r="H88" s="31" t="s">
+        <v>832</v>
+      </c>
       <c r="I88" s="9" t="s">
         <v>282</v>
       </c>
@@ -5709,10 +5749,12 @@
       <c r="F89" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="G89" s="32">
-        <v>0</v>
-      </c>
-      <c r="H89" s="32"/>
+      <c r="G89" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H89" s="31" t="s">
+        <v>837</v>
+      </c>
       <c r="I89" s="9" t="s">
         <v>285</v>
       </c>
@@ -5736,10 +5778,12 @@
       <c r="F90" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="G90" s="32">
-        <v>0</v>
-      </c>
-      <c r="H90" s="32"/>
+      <c r="G90" s="31">
+        <v>4</v>
+      </c>
+      <c r="H90" s="31" t="s">
+        <v>832</v>
+      </c>
       <c r="I90" s="9" t="s">
         <v>288</v>
       </c>
@@ -5763,10 +5807,12 @@
       <c r="F91" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="G91" s="32">
-        <v>0</v>
-      </c>
-      <c r="H91" s="32"/>
+      <c r="G91" s="31">
+        <v>6</v>
+      </c>
+      <c r="H91" s="31" t="s">
+        <v>841</v>
+      </c>
       <c r="I91" s="9" t="s">
         <v>291</v>
       </c>
@@ -5790,10 +5836,12 @@
       <c r="F92" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="G92" s="32">
-        <v>0</v>
-      </c>
-      <c r="H92" s="32"/>
+      <c r="G92" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H92" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I92" s="9" t="s">
         <v>295</v>
       </c>
@@ -5817,10 +5865,12 @@
       <c r="F93" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="G93" s="32">
-        <v>0</v>
-      </c>
-      <c r="H93" s="32"/>
+      <c r="G93" s="31">
+        <v>4</v>
+      </c>
+      <c r="H93" s="31" t="s">
+        <v>841</v>
+      </c>
       <c r="I93" s="9" t="s">
         <v>298</v>
       </c>
@@ -5844,10 +5894,12 @@
       <c r="F94" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="G94" s="32">
-        <v>0</v>
-      </c>
-      <c r="H94" s="32"/>
+      <c r="G94" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H94" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I94" s="9" t="s">
         <v>301</v>
       </c>
@@ -5871,10 +5923,12 @@
       <c r="F95" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="G95" s="32">
-        <v>0</v>
-      </c>
-      <c r="H95" s="32"/>
+      <c r="G95" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H95" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I95" s="9" t="s">
         <v>304</v>
       </c>
@@ -5898,10 +5952,12 @@
       <c r="F96" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="G96" s="32">
-        <v>0</v>
-      </c>
-      <c r="H96" s="32"/>
+      <c r="G96" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H96" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I96" s="9" t="s">
         <v>307</v>
       </c>
@@ -5925,10 +5981,12 @@
       <c r="F97" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="G97" s="32">
-        <v>0</v>
-      </c>
-      <c r="H97" s="32"/>
+      <c r="G97" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H97" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I97" s="9" t="s">
         <v>310</v>
       </c>
@@ -5952,10 +6010,12 @@
       <c r="F98" s="9" t="s">
         <v>312</v>
       </c>
-      <c r="G98" s="32">
-        <v>0</v>
-      </c>
-      <c r="H98" s="32"/>
+      <c r="G98" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H98" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I98" s="9" t="s">
         <v>313</v>
       </c>
@@ -5979,10 +6039,12 @@
       <c r="F99" s="9" t="s">
         <v>315</v>
       </c>
-      <c r="G99" s="32">
-        <v>0</v>
-      </c>
-      <c r="H99" s="32"/>
+      <c r="G99" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H99" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I99" s="9" t="s">
         <v>316</v>
       </c>
@@ -6006,10 +6068,12 @@
       <c r="F100" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="G100" s="32">
-        <v>0</v>
-      </c>
-      <c r="H100" s="32"/>
+      <c r="G100" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H100" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I100" s="9" t="s">
         <v>319</v>
       </c>
@@ -6033,10 +6097,12 @@
       <c r="F101" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="G101" s="32">
-        <v>0</v>
-      </c>
-      <c r="H101" s="32"/>
+      <c r="G101" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H101" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I101" s="9" t="s">
         <v>322</v>
       </c>
@@ -6060,10 +6126,12 @@
       <c r="F102" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="G102" s="32">
-        <v>0</v>
-      </c>
-      <c r="H102" s="32"/>
+      <c r="G102" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H102" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I102" s="9" t="s">
         <v>325</v>
       </c>
@@ -6087,10 +6155,12 @@
       <c r="F103" s="9" t="s">
         <v>327</v>
       </c>
-      <c r="G103" s="32">
-        <v>0</v>
-      </c>
-      <c r="H103" s="32"/>
+      <c r="G103" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H103" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I103" s="9" t="s">
         <v>328</v>
       </c>
@@ -6114,10 +6184,12 @@
       <c r="F104" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="G104" s="32">
-        <v>0</v>
-      </c>
-      <c r="H104" s="32"/>
+      <c r="G104" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H104" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I104" s="9" t="s">
         <v>331</v>
       </c>
@@ -6141,10 +6213,12 @@
       <c r="F105" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="G105" s="32">
-        <v>0</v>
-      </c>
-      <c r="H105" s="32"/>
+      <c r="G105" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H105" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I105" s="9" t="s">
         <v>334</v>
       </c>
@@ -6168,10 +6242,12 @@
       <c r="F106" s="9" t="s">
         <v>336</v>
       </c>
-      <c r="G106" s="32">
-        <v>0</v>
-      </c>
-      <c r="H106" s="32"/>
+      <c r="G106" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H106" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I106" s="9" t="s">
         <v>337</v>
       </c>
@@ -6195,10 +6271,12 @@
       <c r="F107" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="G107" s="32">
-        <v>0</v>
-      </c>
-      <c r="H107" s="32"/>
+      <c r="G107" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H107" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I107" s="9" t="s">
         <v>340</v>
       </c>
@@ -6222,10 +6300,12 @@
       <c r="F108" s="9" t="s">
         <v>342</v>
       </c>
-      <c r="G108" s="32">
-        <v>0</v>
-      </c>
-      <c r="H108" s="32"/>
+      <c r="G108" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H108" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I108" s="9" t="s">
         <v>343</v>
       </c>
@@ -6249,10 +6329,12 @@
       <c r="F109" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="G109" s="32">
-        <v>0</v>
-      </c>
-      <c r="H109" s="32"/>
+      <c r="G109" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H109" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I109" s="9" t="s">
         <v>346</v>
       </c>
@@ -6276,10 +6358,12 @@
       <c r="F110" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="G110" s="32">
-        <v>0</v>
-      </c>
-      <c r="H110" s="32"/>
+      <c r="G110" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H110" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I110" s="9" t="s">
         <v>349</v>
       </c>
@@ -6303,10 +6387,12 @@
       <c r="F111" s="9" t="s">
         <v>351</v>
       </c>
-      <c r="G111" s="32">
-        <v>0</v>
-      </c>
-      <c r="H111" s="32"/>
+      <c r="G111" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H111" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I111" s="9" t="s">
         <v>352</v>
       </c>
@@ -6330,10 +6416,12 @@
       <c r="F112" s="9" t="s">
         <v>354</v>
       </c>
-      <c r="G112" s="32">
-        <v>0</v>
-      </c>
-      <c r="H112" s="32"/>
+      <c r="G112" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H112" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I112" s="9" t="s">
         <v>355</v>
       </c>
@@ -6357,10 +6445,12 @@
       <c r="F113" s="9" t="s">
         <v>357</v>
       </c>
-      <c r="G113" s="32">
-        <v>0</v>
-      </c>
-      <c r="H113" s="32"/>
+      <c r="G113" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H113" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I113" s="9" t="s">
         <v>358</v>
       </c>
@@ -6384,10 +6474,12 @@
       <c r="F114" s="9" t="s">
         <v>360</v>
       </c>
-      <c r="G114" s="32">
-        <v>0</v>
-      </c>
-      <c r="H114" s="32"/>
+      <c r="G114" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H114" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I114" s="9" t="s">
         <v>361</v>
       </c>
@@ -6411,10 +6503,12 @@
       <c r="F115" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="G115" s="32">
-        <v>0</v>
-      </c>
-      <c r="H115" s="32"/>
+      <c r="G115" s="31">
+        <v>-1</v>
+      </c>
+      <c r="H115" s="31" t="s">
+        <v>850</v>
+      </c>
       <c r="I115" s="9" t="s">
         <v>364</v>
       </c>
@@ -6438,10 +6532,12 @@
       <c r="F116" s="9" t="s">
         <v>367</v>
       </c>
-      <c r="G116" s="32">
-        <v>0</v>
-      </c>
-      <c r="H116" s="32"/>
+      <c r="G116" s="31">
+        <v>4</v>
+      </c>
+      <c r="H116" s="31" t="s">
+        <v>841</v>
+      </c>
       <c r="I116" s="9" t="s">
         <v>368</v>
       </c>
@@ -6465,10 +6561,12 @@
       <c r="F117" s="9" t="s">
         <v>370</v>
       </c>
-      <c r="G117" s="32">
-        <v>0</v>
-      </c>
-      <c r="H117" s="32"/>
+      <c r="G117" s="31">
+        <v>4</v>
+      </c>
+      <c r="H117" s="31" t="s">
+        <v>841</v>
+      </c>
       <c r="I117" s="9" t="s">
         <v>371</v>
       </c>
@@ -6492,10 +6590,12 @@
       <c r="F118" s="9" t="s">
         <v>374</v>
       </c>
-      <c r="G118" s="32">
-        <v>0</v>
-      </c>
-      <c r="H118" s="32"/>
+      <c r="G118" s="31">
+        <v>6</v>
+      </c>
+      <c r="H118" s="31" t="s">
+        <v>832</v>
+      </c>
       <c r="I118" s="9" t="s">
         <v>375</v>
       </c>
@@ -6519,10 +6619,12 @@
       <c r="F119" s="9" t="s">
         <v>378</v>
       </c>
-      <c r="G119" s="32">
-        <v>0</v>
-      </c>
-      <c r="H119" s="32"/>
+      <c r="G119" s="31">
+        <v>6</v>
+      </c>
+      <c r="H119" s="31" t="s">
+        <v>841</v>
+      </c>
       <c r="I119" s="9" t="s">
         <v>379</v>
       </c>
@@ -6546,10 +6648,12 @@
       <c r="F120" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="G120" s="32">
-        <v>0</v>
-      </c>
-      <c r="H120" s="32"/>
+      <c r="G120" s="31">
+        <v>6</v>
+      </c>
+      <c r="H120" s="31" t="s">
+        <v>832</v>
+      </c>
       <c r="I120" s="9" t="s">
         <v>382</v>
       </c>
@@ -6573,10 +6677,10 @@
       <c r="F121" s="9" t="s">
         <v>385</v>
       </c>
-      <c r="G121" s="32">
-        <v>0</v>
-      </c>
-      <c r="H121" s="32"/>
+      <c r="G121" s="31">
+        <v>1</v>
+      </c>
+      <c r="H121" s="31"/>
       <c r="I121" s="9" t="s">
         <v>386</v>
       </c>
@@ -6600,10 +6704,12 @@
       <c r="F122" s="9" t="s">
         <v>389</v>
       </c>
-      <c r="G122" s="32">
-        <v>0</v>
-      </c>
-      <c r="H122" s="32"/>
+      <c r="G122" s="31">
+        <v>6</v>
+      </c>
+      <c r="H122" s="31" t="s">
+        <v>852</v>
+      </c>
       <c r="I122" s="9" t="s">
         <v>390</v>
       </c>
@@ -6627,10 +6733,12 @@
       <c r="F123" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="G123" s="32">
-        <v>0</v>
-      </c>
-      <c r="H123" s="32"/>
+      <c r="G123" s="31">
+        <v>6</v>
+      </c>
+      <c r="H123" s="31" t="s">
+        <v>853</v>
+      </c>
       <c r="I123" s="9" t="s">
         <v>393</v>
       </c>
@@ -6654,10 +6762,12 @@
       <c r="F124" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="G124" s="32">
-        <v>0</v>
-      </c>
-      <c r="H124" s="32"/>
+      <c r="G124" s="31">
+        <v>6</v>
+      </c>
+      <c r="H124" s="31" t="s">
+        <v>841</v>
+      </c>
       <c r="I124" s="9" t="s">
         <v>396</v>
       </c>
@@ -6681,10 +6791,12 @@
       <c r="F125" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="G125" s="32">
-        <v>0</v>
-      </c>
-      <c r="H125" s="32"/>
+      <c r="G125" s="31">
+        <v>4</v>
+      </c>
+      <c r="H125" s="31" t="s">
+        <v>832</v>
+      </c>
       <c r="I125" s="9" t="s">
         <v>399</v>
       </c>
@@ -6708,10 +6820,12 @@
       <c r="F126" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="G126" s="32">
-        <v>0</v>
-      </c>
-      <c r="H126" s="32"/>
+      <c r="G126" s="31">
+        <v>4</v>
+      </c>
+      <c r="H126" s="31" t="s">
+        <v>841</v>
+      </c>
       <c r="I126" s="9" t="s">
         <v>402</v>
       </c>
@@ -6735,10 +6849,12 @@
       <c r="F127" s="9" t="s">
         <v>404</v>
       </c>
-      <c r="G127" s="32">
-        <v>0</v>
-      </c>
-      <c r="H127" s="32"/>
+      <c r="G127" s="31">
+        <v>6</v>
+      </c>
+      <c r="H127" s="31" t="s">
+        <v>832</v>
+      </c>
       <c r="I127" s="9" t="s">
         <v>405</v>
       </c>
@@ -6762,10 +6878,12 @@
       <c r="F128" s="9" t="s">
         <v>407</v>
       </c>
-      <c r="G128" s="32">
-        <v>0</v>
-      </c>
-      <c r="H128" s="32"/>
+      <c r="G128" s="31">
+        <v>4</v>
+      </c>
+      <c r="H128" s="31" t="s">
+        <v>841</v>
+      </c>
       <c r="I128" s="9" t="s">
         <v>408</v>
       </c>
@@ -6789,10 +6907,12 @@
       <c r="F129" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="G129" s="32">
-        <v>0</v>
-      </c>
-      <c r="H129" s="32"/>
+      <c r="G129" s="31">
+        <v>4</v>
+      </c>
+      <c r="H129" s="31" t="s">
+        <v>832</v>
+      </c>
       <c r="I129" s="9" t="s">
         <v>411</v>
       </c>
@@ -6816,10 +6936,12 @@
       <c r="F130" s="9" t="s">
         <v>413</v>
       </c>
-      <c r="G130" s="32">
-        <v>0</v>
-      </c>
-      <c r="H130" s="32"/>
+      <c r="G130" s="31">
+        <v>4</v>
+      </c>
+      <c r="H130" s="31" t="s">
+        <v>832</v>
+      </c>
       <c r="I130" s="9" t="s">
         <v>414</v>
       </c>
@@ -6843,10 +6965,12 @@
       <c r="F131" s="9" t="s">
         <v>416</v>
       </c>
-      <c r="G131" s="32">
-        <v>0</v>
-      </c>
-      <c r="H131" s="32"/>
+      <c r="G131" s="31">
+        <v>4</v>
+      </c>
+      <c r="H131" s="31" t="s">
+        <v>832</v>
+      </c>
       <c r="I131" s="9" t="s">
         <v>417</v>
       </c>
@@ -6870,10 +6994,12 @@
       <c r="F132" s="9" t="s">
         <v>419</v>
       </c>
-      <c r="G132" s="32">
-        <v>0</v>
-      </c>
-      <c r="H132" s="32"/>
+      <c r="G132" s="31">
+        <v>4</v>
+      </c>
+      <c r="H132" s="31" t="s">
+        <v>841</v>
+      </c>
       <c r="I132" s="9" t="s">
         <v>420</v>
       </c>
@@ -6897,10 +7023,12 @@
       <c r="F133" s="9" t="s">
         <v>422</v>
       </c>
-      <c r="G133" s="32">
-        <v>0</v>
-      </c>
-      <c r="H133" s="32"/>
+      <c r="G133" s="31">
+        <v>6</v>
+      </c>
+      <c r="H133" s="31" t="s">
+        <v>832</v>
+      </c>
       <c r="I133" s="9" t="s">
         <v>423</v>
       </c>
@@ -6924,10 +7052,10 @@
       <c r="F134" s="9" t="s">
         <v>426</v>
       </c>
-      <c r="G134" s="32">
-        <v>0</v>
-      </c>
-      <c r="H134" s="32"/>
+      <c r="G134" s="31">
+        <v>0</v>
+      </c>
+      <c r="H134" s="31"/>
       <c r="I134" s="9" t="s">
         <v>427</v>
       </c>
@@ -6951,10 +7079,10 @@
       <c r="F135" s="9" t="s">
         <v>428</v>
       </c>
-      <c r="G135" s="32">
-        <v>0</v>
-      </c>
-      <c r="H135" s="32"/>
+      <c r="G135" s="31">
+        <v>0</v>
+      </c>
+      <c r="H135" s="31"/>
       <c r="I135" s="9" t="s">
         <v>429</v>
       </c>
@@ -6978,10 +7106,10 @@
       <c r="F136" s="9" t="s">
         <v>431</v>
       </c>
-      <c r="G136" s="32">
-        <v>0</v>
-      </c>
-      <c r="H136" s="32"/>
+      <c r="G136" s="31">
+        <v>0</v>
+      </c>
+      <c r="H136" s="31"/>
       <c r="I136" s="9" t="s">
         <v>432</v>
       </c>
@@ -7005,10 +7133,10 @@
       <c r="F137" s="9" t="s">
         <v>434</v>
       </c>
-      <c r="G137" s="32">
-        <v>0</v>
-      </c>
-      <c r="H137" s="32"/>
+      <c r="G137" s="31">
+        <v>0</v>
+      </c>
+      <c r="H137" s="31"/>
       <c r="I137" s="9" t="s">
         <v>435</v>
       </c>
@@ -7032,10 +7160,10 @@
       <c r="F138" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="G138" s="32">
-        <v>0</v>
-      </c>
-      <c r="H138" s="32"/>
+      <c r="G138" s="31">
+        <v>0</v>
+      </c>
+      <c r="H138" s="31"/>
       <c r="I138" s="9" t="s">
         <v>438</v>
       </c>
@@ -7059,10 +7187,10 @@
       <c r="F139" s="9" t="s">
         <v>440</v>
       </c>
-      <c r="G139" s="32">
-        <v>0</v>
-      </c>
-      <c r="H139" s="32"/>
+      <c r="G139" s="31">
+        <v>0</v>
+      </c>
+      <c r="H139" s="31"/>
       <c r="I139" s="9" t="s">
         <v>441</v>
       </c>
@@ -7086,10 +7214,10 @@
       <c r="F140" s="9" t="s">
         <v>443</v>
       </c>
-      <c r="G140" s="32">
-        <v>0</v>
-      </c>
-      <c r="H140" s="32"/>
+      <c r="G140" s="31">
+        <v>0</v>
+      </c>
+      <c r="H140" s="31"/>
       <c r="I140" s="9" t="s">
         <v>444</v>
       </c>
@@ -7113,10 +7241,10 @@
       <c r="F141" s="9" t="s">
         <v>446</v>
       </c>
-      <c r="G141" s="32">
-        <v>0</v>
-      </c>
-      <c r="H141" s="32"/>
+      <c r="G141" s="31">
+        <v>0</v>
+      </c>
+      <c r="H141" s="31"/>
       <c r="I141" s="9" t="s">
         <v>447</v>
       </c>
@@ -7140,10 +7268,10 @@
       <c r="F142" s="9" t="s">
         <v>450</v>
       </c>
-      <c r="G142" s="32">
-        <v>0</v>
-      </c>
-      <c r="H142" s="32"/>
+      <c r="G142" s="31">
+        <v>0</v>
+      </c>
+      <c r="H142" s="31"/>
       <c r="I142" s="9" t="s">
         <v>451</v>
       </c>
@@ -7167,10 +7295,10 @@
       <c r="F143" s="9" t="s">
         <v>454</v>
       </c>
-      <c r="G143" s="32">
-        <v>0</v>
-      </c>
-      <c r="H143" s="32"/>
+      <c r="G143" s="31">
+        <v>0</v>
+      </c>
+      <c r="H143" s="31"/>
       <c r="I143" s="9" t="s">
         <v>455</v>
       </c>
@@ -7194,10 +7322,10 @@
       <c r="F144" s="9" t="s">
         <v>458</v>
       </c>
-      <c r="G144" s="32">
-        <v>0</v>
-      </c>
-      <c r="H144" s="32"/>
+      <c r="G144" s="31">
+        <v>0</v>
+      </c>
+      <c r="H144" s="31"/>
       <c r="I144" s="9" t="s">
         <v>459</v>
       </c>
@@ -7221,10 +7349,10 @@
       <c r="F145" s="9" t="s">
         <v>461</v>
       </c>
-      <c r="G145" s="32">
-        <v>0</v>
-      </c>
-      <c r="H145" s="32"/>
+      <c r="G145" s="31">
+        <v>0</v>
+      </c>
+      <c r="H145" s="31"/>
       <c r="I145" s="9" t="s">
         <v>462</v>
       </c>
@@ -7248,10 +7376,10 @@
       <c r="F146" s="9" t="s">
         <v>464</v>
       </c>
-      <c r="G146" s="32">
-        <v>0</v>
-      </c>
-      <c r="H146" s="32"/>
+      <c r="G146" s="31">
+        <v>0</v>
+      </c>
+      <c r="H146" s="31"/>
       <c r="I146" s="9" t="s">
         <v>465</v>
       </c>
@@ -7275,10 +7403,10 @@
       <c r="F147" s="9" t="s">
         <v>467</v>
       </c>
-      <c r="G147" s="32">
-        <v>0</v>
-      </c>
-      <c r="H147" s="32"/>
+      <c r="G147" s="31">
+        <v>0</v>
+      </c>
+      <c r="H147" s="31"/>
       <c r="I147" s="9" t="s">
         <v>468</v>
       </c>
@@ -7302,10 +7430,10 @@
       <c r="F148" s="9" t="s">
         <v>470</v>
       </c>
-      <c r="G148" s="32">
-        <v>0</v>
-      </c>
-      <c r="H148" s="32"/>
+      <c r="G148" s="31">
+        <v>0</v>
+      </c>
+      <c r="H148" s="31"/>
       <c r="I148" s="9" t="s">
         <v>471</v>
       </c>
@@ -7329,10 +7457,10 @@
       <c r="F149" s="9" t="s">
         <v>473</v>
       </c>
-      <c r="G149" s="32">
-        <v>0</v>
-      </c>
-      <c r="H149" s="32"/>
+      <c r="G149" s="31">
+        <v>0</v>
+      </c>
+      <c r="H149" s="31"/>
       <c r="I149" s="9" t="s">
         <v>474</v>
       </c>
@@ -7356,10 +7484,10 @@
       <c r="F150" s="9" t="s">
         <v>477</v>
       </c>
-      <c r="G150" s="32">
-        <v>0</v>
-      </c>
-      <c r="H150" s="32"/>
+      <c r="G150" s="31">
+        <v>0</v>
+      </c>
+      <c r="H150" s="31"/>
       <c r="I150" s="9" t="s">
         <v>478</v>
       </c>
@@ -7383,10 +7511,10 @@
       <c r="F151" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="G151" s="32">
-        <v>0</v>
-      </c>
-      <c r="H151" s="32"/>
+      <c r="G151" s="31">
+        <v>0</v>
+      </c>
+      <c r="H151" s="31"/>
       <c r="I151" s="9" t="s">
         <v>481</v>
       </c>
@@ -7410,10 +7538,10 @@
       <c r="F152" s="9" t="s">
         <v>483</v>
       </c>
-      <c r="G152" s="32">
-        <v>0</v>
-      </c>
-      <c r="H152" s="32"/>
+      <c r="G152" s="31">
+        <v>0</v>
+      </c>
+      <c r="H152" s="31"/>
       <c r="I152" s="9" t="s">
         <v>484</v>
       </c>
@@ -7437,10 +7565,10 @@
       <c r="F153" s="9" t="s">
         <v>486</v>
       </c>
-      <c r="G153" s="32">
-        <v>0</v>
-      </c>
-      <c r="H153" s="32"/>
+      <c r="G153" s="31">
+        <v>0</v>
+      </c>
+      <c r="H153" s="31"/>
       <c r="I153" s="9" t="s">
         <v>487</v>
       </c>
@@ -7464,10 +7592,10 @@
       <c r="F154" s="9" t="s">
         <v>489</v>
       </c>
-      <c r="G154" s="32">
-        <v>0</v>
-      </c>
-      <c r="H154" s="32"/>
+      <c r="G154" s="31">
+        <v>0</v>
+      </c>
+      <c r="H154" s="31"/>
       <c r="I154" s="9" t="s">
         <v>490</v>
       </c>
@@ -7491,10 +7619,10 @@
       <c r="F155" s="9" t="s">
         <v>492</v>
       </c>
-      <c r="G155" s="32">
-        <v>0</v>
-      </c>
-      <c r="H155" s="32"/>
+      <c r="G155" s="31">
+        <v>0</v>
+      </c>
+      <c r="H155" s="31"/>
       <c r="I155" s="9" t="s">
         <v>493</v>
       </c>
@@ -7518,10 +7646,10 @@
       <c r="F156" s="9" t="s">
         <v>494</v>
       </c>
-      <c r="G156" s="32">
-        <v>0</v>
-      </c>
-      <c r="H156" s="32"/>
+      <c r="G156" s="31">
+        <v>0</v>
+      </c>
+      <c r="H156" s="31"/>
       <c r="I156" s="9" t="s">
         <v>495</v>
       </c>
@@ -7545,10 +7673,10 @@
       <c r="F157" s="9" t="s">
         <v>497</v>
       </c>
-      <c r="G157" s="32">
-        <v>0</v>
-      </c>
-      <c r="H157" s="32"/>
+      <c r="G157" s="31">
+        <v>0</v>
+      </c>
+      <c r="H157" s="31"/>
       <c r="I157" s="9" t="s">
         <v>498</v>
       </c>
@@ -7572,10 +7700,10 @@
       <c r="F158" s="9" t="s">
         <v>500</v>
       </c>
-      <c r="G158" s="32">
-        <v>0</v>
-      </c>
-      <c r="H158" s="32"/>
+      <c r="G158" s="31">
+        <v>0</v>
+      </c>
+      <c r="H158" s="31"/>
       <c r="I158" s="9" t="s">
         <v>501</v>
       </c>
@@ -7599,10 +7727,10 @@
       <c r="F159" s="9" t="s">
         <v>503</v>
       </c>
-      <c r="G159" s="32">
-        <v>0</v>
-      </c>
-      <c r="H159" s="32"/>
+      <c r="G159" s="31">
+        <v>0</v>
+      </c>
+      <c r="H159" s="31"/>
       <c r="I159" s="9" t="s">
         <v>504</v>
       </c>
@@ -7626,10 +7754,10 @@
       <c r="F160" s="9" t="s">
         <v>506</v>
       </c>
-      <c r="G160" s="32">
-        <v>0</v>
-      </c>
-      <c r="H160" s="32"/>
+      <c r="G160" s="31">
+        <v>0</v>
+      </c>
+      <c r="H160" s="31"/>
       <c r="I160" s="9" t="s">
         <v>507</v>
       </c>
@@ -7653,10 +7781,10 @@
       <c r="F161" s="9" t="s">
         <v>509</v>
       </c>
-      <c r="G161" s="32">
-        <v>0</v>
-      </c>
-      <c r="H161" s="32"/>
+      <c r="G161" s="31">
+        <v>0</v>
+      </c>
+      <c r="H161" s="31"/>
       <c r="I161" s="9" t="s">
         <v>510</v>
       </c>
@@ -7680,10 +7808,10 @@
       <c r="F162" s="9" t="s">
         <v>512</v>
       </c>
-      <c r="G162" s="32">
-        <v>0</v>
-      </c>
-      <c r="H162" s="32"/>
+      <c r="G162" s="31">
+        <v>0</v>
+      </c>
+      <c r="H162" s="31"/>
       <c r="I162" s="9" t="s">
         <v>513</v>
       </c>
@@ -7707,10 +7835,10 @@
       <c r="F163" s="9" t="s">
         <v>515</v>
       </c>
-      <c r="G163" s="32">
-        <v>0</v>
-      </c>
-      <c r="H163" s="32"/>
+      <c r="G163" s="31">
+        <v>0</v>
+      </c>
+      <c r="H163" s="31"/>
       <c r="I163" s="9" t="s">
         <v>516</v>
       </c>
@@ -7734,10 +7862,10 @@
       <c r="F164" s="9" t="s">
         <v>506</v>
       </c>
-      <c r="G164" s="32">
-        <v>0</v>
-      </c>
-      <c r="H164" s="32"/>
+      <c r="G164" s="31">
+        <v>0</v>
+      </c>
+      <c r="H164" s="31"/>
       <c r="I164" s="9" t="s">
         <v>518</v>
       </c>
@@ -7761,10 +7889,10 @@
       <c r="F165" s="9" t="s">
         <v>520</v>
       </c>
-      <c r="G165" s="32">
-        <v>0</v>
-      </c>
-      <c r="H165" s="32"/>
+      <c r="G165" s="31">
+        <v>0</v>
+      </c>
+      <c r="H165" s="31"/>
       <c r="I165" s="9" t="s">
         <v>521</v>
       </c>
@@ -7788,10 +7916,10 @@
       <c r="F166" s="9" t="s">
         <v>523</v>
       </c>
-      <c r="G166" s="32">
-        <v>0</v>
-      </c>
-      <c r="H166" s="32"/>
+      <c r="G166" s="31">
+        <v>0</v>
+      </c>
+      <c r="H166" s="31"/>
       <c r="I166" s="9" t="s">
         <v>524</v>
       </c>
@@ -7815,10 +7943,10 @@
       <c r="F167" s="9" t="s">
         <v>526</v>
       </c>
-      <c r="G167" s="32">
-        <v>0</v>
-      </c>
-      <c r="H167" s="32"/>
+      <c r="G167" s="31">
+        <v>0</v>
+      </c>
+      <c r="H167" s="31"/>
       <c r="I167" s="9" t="s">
         <v>527</v>
       </c>
@@ -7842,10 +7970,10 @@
       <c r="F168" s="9" t="s">
         <v>529</v>
       </c>
-      <c r="G168" s="32">
-        <v>0</v>
-      </c>
-      <c r="H168" s="32"/>
+      <c r="G168" s="31">
+        <v>0</v>
+      </c>
+      <c r="H168" s="31"/>
       <c r="I168" s="9" t="s">
         <v>530</v>
       </c>
@@ -7869,10 +7997,10 @@
       <c r="F169" s="9" t="s">
         <v>532</v>
       </c>
-      <c r="G169" s="32">
-        <v>0</v>
-      </c>
-      <c r="H169" s="32"/>
+      <c r="G169" s="31">
+        <v>0</v>
+      </c>
+      <c r="H169" s="31"/>
       <c r="I169" s="9" t="s">
         <v>533</v>
       </c>
@@ -7896,10 +8024,10 @@
       <c r="F170" s="9" t="s">
         <v>535</v>
       </c>
-      <c r="G170" s="32">
-        <v>0</v>
-      </c>
-      <c r="H170" s="32"/>
+      <c r="G170" s="31">
+        <v>0</v>
+      </c>
+      <c r="H170" s="31"/>
       <c r="I170" s="9" t="s">
         <v>536</v>
       </c>
@@ -7923,10 +8051,10 @@
       <c r="F171" s="9" t="s">
         <v>538</v>
       </c>
-      <c r="G171" s="32">
-        <v>0</v>
-      </c>
-      <c r="H171" s="32"/>
+      <c r="G171" s="31">
+        <v>0</v>
+      </c>
+      <c r="H171" s="31"/>
       <c r="I171" s="9" t="s">
         <v>539</v>
       </c>
@@ -7950,10 +8078,10 @@
       <c r="F172" s="9" t="s">
         <v>541</v>
       </c>
-      <c r="G172" s="32">
-        <v>0</v>
-      </c>
-      <c r="H172" s="32"/>
+      <c r="G172" s="31">
+        <v>0</v>
+      </c>
+      <c r="H172" s="31"/>
       <c r="I172" s="9" t="s">
         <v>542</v>
       </c>
@@ -7977,10 +8105,10 @@
       <c r="F173" s="9" t="s">
         <v>543</v>
       </c>
-      <c r="G173" s="32">
-        <v>0</v>
-      </c>
-      <c r="H173" s="32"/>
+      <c r="G173" s="31">
+        <v>0</v>
+      </c>
+      <c r="H173" s="31"/>
       <c r="I173" s="9" t="s">
         <v>544</v>
       </c>
@@ -8004,10 +8132,10 @@
       <c r="F174" s="9" t="s">
         <v>546</v>
       </c>
-      <c r="G174" s="32">
-        <v>0</v>
-      </c>
-      <c r="H174" s="32"/>
+      <c r="G174" s="31">
+        <v>0</v>
+      </c>
+      <c r="H174" s="31"/>
       <c r="I174" s="9" t="s">
         <v>547</v>
       </c>
@@ -8031,10 +8159,10 @@
       <c r="F175" s="9" t="s">
         <v>549</v>
       </c>
-      <c r="G175" s="32">
-        <v>0</v>
-      </c>
-      <c r="H175" s="32"/>
+      <c r="G175" s="31">
+        <v>0</v>
+      </c>
+      <c r="H175" s="31"/>
       <c r="I175" s="9" t="s">
         <v>550</v>
       </c>
@@ -8058,10 +8186,10 @@
       <c r="F176" s="9" t="s">
         <v>552</v>
       </c>
-      <c r="G176" s="32">
-        <v>0</v>
-      </c>
-      <c r="H176" s="32"/>
+      <c r="G176" s="31">
+        <v>0</v>
+      </c>
+      <c r="H176" s="31"/>
       <c r="I176" s="9" t="s">
         <v>553</v>
       </c>
@@ -8085,10 +8213,10 @@
       <c r="F177" s="9" t="s">
         <v>555</v>
       </c>
-      <c r="G177" s="32">
-        <v>0</v>
-      </c>
-      <c r="H177" s="32"/>
+      <c r="G177" s="31">
+        <v>0</v>
+      </c>
+      <c r="H177" s="31"/>
       <c r="I177" s="9" t="s">
         <v>556</v>
       </c>
@@ -8112,10 +8240,10 @@
       <c r="F178" s="9" t="s">
         <v>559</v>
       </c>
-      <c r="G178" s="32">
-        <v>0</v>
-      </c>
-      <c r="H178" s="32"/>
+      <c r="G178" s="31">
+        <v>0</v>
+      </c>
+      <c r="H178" s="31"/>
       <c r="I178" s="9" t="s">
         <v>560</v>
       </c>
@@ -8139,10 +8267,10 @@
       <c r="F179" s="9" t="s">
         <v>562</v>
       </c>
-      <c r="G179" s="32">
-        <v>0</v>
-      </c>
-      <c r="H179" s="32"/>
+      <c r="G179" s="31">
+        <v>0</v>
+      </c>
+      <c r="H179" s="31"/>
       <c r="I179" s="9" t="s">
         <v>563</v>
       </c>
@@ -8166,10 +8294,10 @@
       <c r="F180" s="9" t="s">
         <v>565</v>
       </c>
-      <c r="G180" s="32">
-        <v>0</v>
-      </c>
-      <c r="H180" s="32"/>
+      <c r="G180" s="31">
+        <v>0</v>
+      </c>
+      <c r="H180" s="31"/>
       <c r="I180" s="9" t="s">
         <v>566</v>
       </c>
@@ -8193,10 +8321,10 @@
       <c r="F181" s="9" t="s">
         <v>477</v>
       </c>
-      <c r="G181" s="32">
-        <v>0</v>
-      </c>
-      <c r="H181" s="32"/>
+      <c r="G181" s="31">
+        <v>0</v>
+      </c>
+      <c r="H181" s="31"/>
       <c r="I181" s="9" t="s">
         <v>568</v>
       </c>
@@ -8220,10 +8348,10 @@
       <c r="F182" s="9" t="s">
         <v>458</v>
       </c>
-      <c r="G182" s="32">
-        <v>0</v>
-      </c>
-      <c r="H182" s="32"/>
+      <c r="G182" s="31">
+        <v>0</v>
+      </c>
+      <c r="H182" s="31"/>
       <c r="I182" s="9" t="s">
         <v>459</v>
       </c>
@@ -8247,10 +8375,10 @@
       <c r="F183" s="9" t="s">
         <v>486</v>
       </c>
-      <c r="G183" s="32">
-        <v>0</v>
-      </c>
-      <c r="H183" s="32"/>
+      <c r="G183" s="31">
+        <v>0</v>
+      </c>
+      <c r="H183" s="31"/>
       <c r="I183" s="9" t="s">
         <v>487</v>
       </c>
@@ -8274,10 +8402,10 @@
       <c r="F184" s="9" t="s">
         <v>570</v>
       </c>
-      <c r="G184" s="32">
-        <v>0</v>
-      </c>
-      <c r="H184" s="32"/>
+      <c r="G184" s="31">
+        <v>0</v>
+      </c>
+      <c r="H184" s="31"/>
       <c r="I184" s="9" t="s">
         <v>571</v>
       </c>
@@ -8301,10 +8429,10 @@
       <c r="F185" s="9" t="s">
         <v>483</v>
       </c>
-      <c r="G185" s="32">
-        <v>0</v>
-      </c>
-      <c r="H185" s="32"/>
+      <c r="G185" s="31">
+        <v>0</v>
+      </c>
+      <c r="H185" s="31"/>
       <c r="I185" s="9" t="s">
         <v>572</v>
       </c>
@@ -8328,10 +8456,10 @@
       <c r="F186" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="G186" s="32">
-        <v>0</v>
-      </c>
-      <c r="H186" s="32"/>
+      <c r="G186" s="31">
+        <v>0</v>
+      </c>
+      <c r="H186" s="31"/>
       <c r="I186" s="9" t="s">
         <v>481</v>
       </c>
@@ -8355,10 +8483,10 @@
       <c r="F187" s="9" t="s">
         <v>489</v>
       </c>
-      <c r="G187" s="32">
-        <v>0</v>
-      </c>
-      <c r="H187" s="32"/>
+      <c r="G187" s="31">
+        <v>0</v>
+      </c>
+      <c r="H187" s="31"/>
       <c r="I187" s="9" t="s">
         <v>573</v>
       </c>
@@ -8382,10 +8510,10 @@
       <c r="F188" s="9" t="s">
         <v>461</v>
       </c>
-      <c r="G188" s="32">
-        <v>0</v>
-      </c>
-      <c r="H188" s="32"/>
+      <c r="G188" s="31">
+        <v>0</v>
+      </c>
+      <c r="H188" s="31"/>
       <c r="I188" s="9" t="s">
         <v>574</v>
       </c>
@@ -8409,10 +8537,10 @@
       <c r="F189" s="9" t="s">
         <v>576</v>
       </c>
-      <c r="G189" s="32">
-        <v>0</v>
-      </c>
-      <c r="H189" s="32"/>
+      <c r="G189" s="31">
+        <v>0</v>
+      </c>
+      <c r="H189" s="31"/>
       <c r="I189" s="9" t="s">
         <v>577</v>
       </c>
@@ -8436,10 +8564,10 @@
       <c r="F190" s="9" t="s">
         <v>579</v>
       </c>
-      <c r="G190" s="32">
-        <v>0</v>
-      </c>
-      <c r="H190" s="32"/>
+      <c r="G190" s="31">
+        <v>0</v>
+      </c>
+      <c r="H190" s="31"/>
       <c r="I190" s="9" t="s">
         <v>580</v>
       </c>
@@ -8463,10 +8591,10 @@
       <c r="F191" s="9" t="s">
         <v>582</v>
       </c>
-      <c r="G191" s="32">
-        <v>0</v>
-      </c>
-      <c r="H191" s="32"/>
+      <c r="G191" s="31">
+        <v>0</v>
+      </c>
+      <c r="H191" s="31"/>
       <c r="I191" s="9" t="s">
         <v>583</v>
       </c>
@@ -8490,10 +8618,10 @@
       <c r="F192" s="9" t="s">
         <v>497</v>
       </c>
-      <c r="G192" s="32">
-        <v>0</v>
-      </c>
-      <c r="H192" s="32"/>
+      <c r="G192" s="31">
+        <v>0</v>
+      </c>
+      <c r="H192" s="31"/>
       <c r="I192" s="9" t="s">
         <v>498</v>
       </c>
@@ -8517,10 +8645,10 @@
       <c r="F193" s="9" t="s">
         <v>585</v>
       </c>
-      <c r="G193" s="32">
-        <v>0</v>
-      </c>
-      <c r="H193" s="32"/>
+      <c r="G193" s="31">
+        <v>0</v>
+      </c>
+      <c r="H193" s="31"/>
       <c r="I193" s="9" t="s">
         <v>586</v>
       </c>
@@ -8544,10 +8672,10 @@
       <c r="F194" s="9" t="s">
         <v>464</v>
       </c>
-      <c r="G194" s="32">
-        <v>0</v>
-      </c>
-      <c r="H194" s="32"/>
+      <c r="G194" s="31">
+        <v>0</v>
+      </c>
+      <c r="H194" s="31"/>
       <c r="I194" s="9" t="s">
         <v>587</v>
       </c>
@@ -8571,10 +8699,10 @@
       <c r="F195" s="9" t="s">
         <v>494</v>
       </c>
-      <c r="G195" s="32">
-        <v>0</v>
-      </c>
-      <c r="H195" s="32"/>
+      <c r="G195" s="31">
+        <v>0</v>
+      </c>
+      <c r="H195" s="31"/>
       <c r="I195" s="9" t="s">
         <v>588</v>
       </c>
@@ -8598,10 +8726,10 @@
       <c r="F196" s="9" t="s">
         <v>590</v>
       </c>
-      <c r="G196" s="32">
-        <v>0</v>
-      </c>
-      <c r="H196" s="32"/>
+      <c r="G196" s="31">
+        <v>0</v>
+      </c>
+      <c r="H196" s="31"/>
       <c r="I196" s="9" t="s">
         <v>591</v>
       </c>
@@ -8625,10 +8753,10 @@
       <c r="F197" s="9" t="s">
         <v>593</v>
       </c>
-      <c r="G197" s="32">
-        <v>0</v>
-      </c>
-      <c r="H197" s="32"/>
+      <c r="G197" s="31">
+        <v>0</v>
+      </c>
+      <c r="H197" s="31"/>
       <c r="I197" s="9" t="s">
         <v>594</v>
       </c>
@@ -8652,10 +8780,10 @@
       <c r="F198" s="9" t="s">
         <v>596</v>
       </c>
-      <c r="G198" s="32">
-        <v>0</v>
-      </c>
-      <c r="H198" s="32"/>
+      <c r="G198" s="31">
+        <v>0</v>
+      </c>
+      <c r="H198" s="31"/>
       <c r="I198" s="9" t="s">
         <v>597</v>
       </c>
@@ -8679,10 +8807,10 @@
       <c r="F199" s="9" t="s">
         <v>599</v>
       </c>
-      <c r="G199" s="32">
-        <v>0</v>
-      </c>
-      <c r="H199" s="32"/>
+      <c r="G199" s="31">
+        <v>0</v>
+      </c>
+      <c r="H199" s="31"/>
       <c r="I199" s="9" t="s">
         <v>600</v>
       </c>
@@ -8706,10 +8834,10 @@
       <c r="F200" s="9" t="s">
         <v>526</v>
       </c>
-      <c r="G200" s="32">
-        <v>0</v>
-      </c>
-      <c r="H200" s="32"/>
+      <c r="G200" s="31">
+        <v>0</v>
+      </c>
+      <c r="H200" s="31"/>
       <c r="I200" s="9" t="s">
         <v>527</v>
       </c>
@@ -8733,10 +8861,10 @@
       <c r="F201" s="9" t="s">
         <v>602</v>
       </c>
-      <c r="G201" s="32">
-        <v>0</v>
-      </c>
-      <c r="H201" s="32"/>
+      <c r="G201" s="31">
+        <v>0</v>
+      </c>
+      <c r="H201" s="31"/>
       <c r="I201" s="9" t="s">
         <v>603</v>
       </c>
@@ -8760,10 +8888,10 @@
       <c r="F202" s="9" t="s">
         <v>605</v>
       </c>
-      <c r="G202" s="32">
-        <v>0</v>
-      </c>
-      <c r="H202" s="32"/>
+      <c r="G202" s="31">
+        <v>0</v>
+      </c>
+      <c r="H202" s="31"/>
       <c r="I202" s="9" t="s">
         <v>606</v>
       </c>
@@ -8787,10 +8915,10 @@
       <c r="F203" s="9" t="s">
         <v>608</v>
       </c>
-      <c r="G203" s="32">
-        <v>0</v>
-      </c>
-      <c r="H203" s="32"/>
+      <c r="G203" s="31">
+        <v>0</v>
+      </c>
+      <c r="H203" s="31"/>
       <c r="I203" s="9" t="s">
         <v>609</v>
       </c>
@@ -8814,10 +8942,10 @@
       <c r="F204" s="9" t="s">
         <v>467</v>
       </c>
-      <c r="G204" s="32">
-        <v>0</v>
-      </c>
-      <c r="H204" s="32"/>
+      <c r="G204" s="31">
+        <v>0</v>
+      </c>
+      <c r="H204" s="31"/>
       <c r="I204" s="9" t="s">
         <v>468</v>
       </c>
@@ -8841,10 +8969,10 @@
       <c r="F205" s="9" t="s">
         <v>611</v>
       </c>
-      <c r="G205" s="32">
-        <v>0</v>
-      </c>
-      <c r="H205" s="32"/>
+      <c r="G205" s="31">
+        <v>0</v>
+      </c>
+      <c r="H205" s="31"/>
       <c r="I205" s="9" t="s">
         <v>612</v>
       </c>
@@ -8868,10 +8996,10 @@
       <c r="F206" s="9" t="s">
         <v>614</v>
       </c>
-      <c r="G206" s="32">
-        <v>0</v>
-      </c>
-      <c r="H206" s="32"/>
+      <c r="G206" s="31">
+        <v>0</v>
+      </c>
+      <c r="H206" s="31"/>
       <c r="I206" s="9" t="s">
         <v>615</v>
       </c>
@@ -8895,10 +9023,10 @@
       <c r="F207" s="9" t="s">
         <v>617</v>
       </c>
-      <c r="G207" s="32">
-        <v>0</v>
-      </c>
-      <c r="H207" s="32"/>
+      <c r="G207" s="31">
+        <v>0</v>
+      </c>
+      <c r="H207" s="31"/>
       <c r="I207" s="9" t="s">
         <v>618</v>
       </c>
@@ -8922,10 +9050,10 @@
       <c r="F208" s="9" t="s">
         <v>470</v>
       </c>
-      <c r="G208" s="32">
-        <v>0</v>
-      </c>
-      <c r="H208" s="32"/>
+      <c r="G208" s="31">
+        <v>0</v>
+      </c>
+      <c r="H208" s="31"/>
       <c r="I208" s="9" t="s">
         <v>619</v>
       </c>
@@ -8949,10 +9077,10 @@
       <c r="F209" s="9" t="s">
         <v>621</v>
       </c>
-      <c r="G209" s="32">
-        <v>0</v>
-      </c>
-      <c r="H209" s="32"/>
+      <c r="G209" s="31">
+        <v>0</v>
+      </c>
+      <c r="H209" s="31"/>
       <c r="I209" s="9" t="s">
         <v>622</v>
       </c>
@@ -8976,10 +9104,10 @@
       <c r="F210" s="9" t="s">
         <v>624</v>
       </c>
-      <c r="G210" s="32">
-        <v>0</v>
-      </c>
-      <c r="H210" s="32"/>
+      <c r="G210" s="31">
+        <v>0</v>
+      </c>
+      <c r="H210" s="31"/>
       <c r="I210" s="9" t="s">
         <v>625</v>
       </c>
@@ -9003,10 +9131,10 @@
       <c r="F211" s="9" t="s">
         <v>627</v>
       </c>
-      <c r="G211" s="32">
-        <v>0</v>
-      </c>
-      <c r="H211" s="32"/>
+      <c r="G211" s="31">
+        <v>0</v>
+      </c>
+      <c r="H211" s="31"/>
       <c r="I211" s="9" t="s">
         <v>628</v>
       </c>
@@ -9030,10 +9158,10 @@
       <c r="F212" s="9" t="s">
         <v>473</v>
       </c>
-      <c r="G212" s="32">
-        <v>0</v>
-      </c>
-      <c r="H212" s="32"/>
+      <c r="G212" s="31">
+        <v>0</v>
+      </c>
+      <c r="H212" s="31"/>
       <c r="I212" s="9" t="s">
         <v>629</v>
       </c>
@@ -9057,10 +9185,10 @@
       <c r="F213" s="9" t="s">
         <v>631</v>
       </c>
-      <c r="G213" s="32">
-        <v>0</v>
-      </c>
-      <c r="H213" s="32"/>
+      <c r="G213" s="31">
+        <v>0</v>
+      </c>
+      <c r="H213" s="31"/>
       <c r="I213" s="9" t="s">
         <v>632</v>
       </c>
@@ -9084,10 +9212,10 @@
       <c r="F214" s="9" t="s">
         <v>634</v>
       </c>
-      <c r="G214" s="32">
-        <v>0</v>
-      </c>
-      <c r="H214" s="32"/>
+      <c r="G214" s="31">
+        <v>0</v>
+      </c>
+      <c r="H214" s="31"/>
       <c r="I214" s="9" t="s">
         <v>635</v>
       </c>
@@ -9111,10 +9239,10 @@
       <c r="F215" s="9" t="s">
         <v>637</v>
       </c>
-      <c r="G215" s="32">
-        <v>0</v>
-      </c>
-      <c r="H215" s="32"/>
+      <c r="G215" s="31">
+        <v>0</v>
+      </c>
+      <c r="H215" s="31"/>
       <c r="I215" s="9" t="s">
         <v>638</v>
       </c>
@@ -9138,10 +9266,10 @@
       <c r="F216" s="9" t="s">
         <v>640</v>
       </c>
-      <c r="G216" s="32">
-        <v>0</v>
-      </c>
-      <c r="H216" s="32"/>
+      <c r="G216" s="31">
+        <v>0</v>
+      </c>
+      <c r="H216" s="31"/>
       <c r="I216" s="9" t="s">
         <v>641</v>
       </c>
@@ -9165,10 +9293,10 @@
       <c r="F217" s="9" t="s">
         <v>643</v>
       </c>
-      <c r="G217" s="32">
-        <v>0</v>
-      </c>
-      <c r="H217" s="32"/>
+      <c r="G217" s="31">
+        <v>0</v>
+      </c>
+      <c r="H217" s="31"/>
       <c r="I217" s="9" t="s">
         <v>644</v>
       </c>
@@ -9192,10 +9320,10 @@
       <c r="F218" s="9" t="s">
         <v>647</v>
       </c>
-      <c r="G218" s="32">
-        <v>0</v>
-      </c>
-      <c r="H218" s="32"/>
+      <c r="G218" s="31">
+        <v>0</v>
+      </c>
+      <c r="H218" s="31"/>
       <c r="I218" s="9" t="s">
         <v>648</v>
       </c>
@@ -9219,10 +9347,10 @@
       <c r="F219" s="9" t="s">
         <v>650</v>
       </c>
-      <c r="G219" s="32">
-        <v>0</v>
-      </c>
-      <c r="H219" s="32"/>
+      <c r="G219" s="31">
+        <v>0</v>
+      </c>
+      <c r="H219" s="31"/>
       <c r="I219" s="9" t="s">
         <v>651</v>
       </c>
@@ -9246,10 +9374,10 @@
       <c r="F220" s="9" t="s">
         <v>653</v>
       </c>
-      <c r="G220" s="32">
-        <v>0</v>
-      </c>
-      <c r="H220" s="32"/>
+      <c r="G220" s="31">
+        <v>0</v>
+      </c>
+      <c r="H220" s="31"/>
       <c r="I220" s="9" t="s">
         <v>654</v>
       </c>
@@ -9273,10 +9401,10 @@
       <c r="F221" s="9" t="s">
         <v>656</v>
       </c>
-      <c r="G221" s="32">
-        <v>0</v>
-      </c>
-      <c r="H221" s="32"/>
+      <c r="G221" s="31">
+        <v>0</v>
+      </c>
+      <c r="H221" s="31"/>
       <c r="I221" s="9" t="s">
         <v>657</v>
       </c>
@@ -9300,10 +9428,10 @@
       <c r="F222" s="9" t="s">
         <v>660</v>
       </c>
-      <c r="G222" s="32">
-        <v>0</v>
-      </c>
-      <c r="H222" s="32"/>
+      <c r="G222" s="31">
+        <v>0</v>
+      </c>
+      <c r="H222" s="31"/>
       <c r="I222" s="9" t="s">
         <v>661</v>
       </c>
@@ -9327,10 +9455,10 @@
       <c r="F223" s="9" t="s">
         <v>663</v>
       </c>
-      <c r="G223" s="32">
-        <v>0</v>
-      </c>
-      <c r="H223" s="32"/>
+      <c r="G223" s="31">
+        <v>0</v>
+      </c>
+      <c r="H223" s="31"/>
       <c r="I223" s="9" t="s">
         <v>664</v>
       </c>
@@ -9354,10 +9482,10 @@
       <c r="F224" s="9" t="s">
         <v>666</v>
       </c>
-      <c r="G224" s="32">
-        <v>0</v>
-      </c>
-      <c r="H224" s="32"/>
+      <c r="G224" s="31">
+        <v>0</v>
+      </c>
+      <c r="H224" s="31"/>
       <c r="I224" s="9" t="s">
         <v>667</v>
       </c>
@@ -9381,10 +9509,10 @@
       <c r="F225" s="9" t="s">
         <v>669</v>
       </c>
-      <c r="G225" s="32">
-        <v>0</v>
-      </c>
-      <c r="H225" s="32"/>
+      <c r="G225" s="31">
+        <v>0</v>
+      </c>
+      <c r="H225" s="31"/>
       <c r="I225" s="9" t="s">
         <v>670</v>
       </c>
@@ -9408,10 +9536,10 @@
       <c r="F226" s="9" t="s">
         <v>672</v>
       </c>
-      <c r="G226" s="32">
-        <v>0</v>
-      </c>
-      <c r="H226" s="32"/>
+      <c r="G226" s="31">
+        <v>0</v>
+      </c>
+      <c r="H226" s="31"/>
       <c r="I226" s="9" t="s">
         <v>673</v>
       </c>
@@ -9435,10 +9563,10 @@
       <c r="F227" s="9" t="s">
         <v>675</v>
       </c>
-      <c r="G227" s="32">
-        <v>0</v>
-      </c>
-      <c r="H227" s="32"/>
+      <c r="G227" s="31">
+        <v>0</v>
+      </c>
+      <c r="H227" s="31"/>
       <c r="I227" s="9" t="s">
         <v>676</v>
       </c>
@@ -9462,10 +9590,10 @@
       <c r="F228" s="9" t="s">
         <v>678</v>
       </c>
-      <c r="G228" s="32">
-        <v>0</v>
-      </c>
-      <c r="H228" s="32"/>
+      <c r="G228" s="31">
+        <v>0</v>
+      </c>
+      <c r="H228" s="31"/>
       <c r="I228" s="9" t="s">
         <v>679</v>
       </c>
@@ -9489,10 +9617,10 @@
       <c r="F229" s="9" t="s">
         <v>681</v>
       </c>
-      <c r="G229" s="32">
-        <v>0</v>
-      </c>
-      <c r="H229" s="32"/>
+      <c r="G229" s="31">
+        <v>0</v>
+      </c>
+      <c r="H229" s="31"/>
       <c r="I229" s="9" t="s">
         <v>682</v>
       </c>
@@ -9516,10 +9644,10 @@
       <c r="F230" s="9" t="s">
         <v>684</v>
       </c>
-      <c r="G230" s="32">
-        <v>0</v>
-      </c>
-      <c r="H230" s="32"/>
+      <c r="G230" s="31">
+        <v>0</v>
+      </c>
+      <c r="H230" s="31"/>
       <c r="I230" s="9" t="s">
         <v>685</v>
       </c>
@@ -9543,10 +9671,10 @@
       <c r="F231" s="9" t="s">
         <v>687</v>
       </c>
-      <c r="G231" s="32">
-        <v>0</v>
-      </c>
-      <c r="H231" s="32"/>
+      <c r="G231" s="31">
+        <v>0</v>
+      </c>
+      <c r="H231" s="31"/>
       <c r="I231" s="9" t="s">
         <v>688</v>
       </c>
@@ -9570,10 +9698,10 @@
       <c r="F232" s="9" t="s">
         <v>690</v>
       </c>
-      <c r="G232" s="32">
-        <v>0</v>
-      </c>
-      <c r="H232" s="32"/>
+      <c r="G232" s="31">
+        <v>0</v>
+      </c>
+      <c r="H232" s="31"/>
       <c r="I232" s="9" t="s">
         <v>691</v>
       </c>
@@ -9597,10 +9725,10 @@
       <c r="F233" s="9" t="s">
         <v>693</v>
       </c>
-      <c r="G233" s="32">
-        <v>0</v>
-      </c>
-      <c r="H233" s="32"/>
+      <c r="G233" s="31">
+        <v>0</v>
+      </c>
+      <c r="H233" s="31"/>
       <c r="I233" s="9" t="s">
         <v>694</v>
       </c>
@@ -9624,10 +9752,10 @@
       <c r="F234" s="9" t="s">
         <v>696</v>
       </c>
-      <c r="G234" s="32">
-        <v>0</v>
-      </c>
-      <c r="H234" s="32"/>
+      <c r="G234" s="31">
+        <v>0</v>
+      </c>
+      <c r="H234" s="31"/>
       <c r="I234" s="9" t="s">
         <v>697</v>
       </c>
@@ -9651,10 +9779,10 @@
       <c r="F235" s="9" t="s">
         <v>699</v>
       </c>
-      <c r="G235" s="32">
-        <v>0</v>
-      </c>
-      <c r="H235" s="32"/>
+      <c r="G235" s="31">
+        <v>0</v>
+      </c>
+      <c r="H235" s="31"/>
       <c r="I235" s="9" t="s">
         <v>700</v>
       </c>
@@ -9678,10 +9806,10 @@
       <c r="F236" s="9" t="s">
         <v>702</v>
       </c>
-      <c r="G236" s="32">
-        <v>0</v>
-      </c>
-      <c r="H236" s="32"/>
+      <c r="G236" s="31">
+        <v>0</v>
+      </c>
+      <c r="H236" s="31"/>
       <c r="I236" s="9" t="s">
         <v>703</v>
       </c>
@@ -9705,10 +9833,10 @@
       <c r="F237" s="9" t="s">
         <v>705</v>
       </c>
-      <c r="G237" s="32">
-        <v>0</v>
-      </c>
-      <c r="H237" s="32"/>
+      <c r="G237" s="31">
+        <v>0</v>
+      </c>
+      <c r="H237" s="31"/>
       <c r="I237" s="9" t="s">
         <v>706</v>
       </c>
@@ -9732,10 +9860,10 @@
       <c r="F238" s="9" t="s">
         <v>709</v>
       </c>
-      <c r="G238" s="32">
-        <v>0</v>
-      </c>
-      <c r="H238" s="32"/>
+      <c r="G238" s="31">
+        <v>0</v>
+      </c>
+      <c r="H238" s="31"/>
       <c r="I238" s="9" t="s">
         <v>710</v>
       </c>
@@ -9759,10 +9887,10 @@
       <c r="F239" s="9" t="s">
         <v>712</v>
       </c>
-      <c r="G239" s="32">
-        <v>0</v>
-      </c>
-      <c r="H239" s="32"/>
+      <c r="G239" s="31">
+        <v>0</v>
+      </c>
+      <c r="H239" s="31"/>
       <c r="I239" s="9" t="s">
         <v>713</v>
       </c>
@@ -9786,10 +9914,10 @@
       <c r="F240" s="9" t="s">
         <v>715</v>
       </c>
-      <c r="G240" s="32">
-        <v>0</v>
-      </c>
-      <c r="H240" s="32"/>
+      <c r="G240" s="31">
+        <v>0</v>
+      </c>
+      <c r="H240" s="31"/>
       <c r="I240" s="9" t="s">
         <v>716</v>
       </c>
@@ -9813,10 +9941,10 @@
       <c r="F241" s="9" t="s">
         <v>718</v>
       </c>
-      <c r="G241" s="32">
-        <v>0</v>
-      </c>
-      <c r="H241" s="32"/>
+      <c r="G241" s="31">
+        <v>0</v>
+      </c>
+      <c r="H241" s="31"/>
       <c r="I241" s="9" t="s">
         <v>719</v>
       </c>
@@ -9840,10 +9968,10 @@
       <c r="F242" s="9" t="s">
         <v>721</v>
       </c>
-      <c r="G242" s="32">
-        <v>0</v>
-      </c>
-      <c r="H242" s="32"/>
+      <c r="G242" s="31">
+        <v>0</v>
+      </c>
+      <c r="H242" s="31"/>
       <c r="I242" s="9" t="s">
         <v>722</v>
       </c>
@@ -9867,10 +9995,10 @@
       <c r="F243" s="9" t="s">
         <v>724</v>
       </c>
-      <c r="G243" s="32">
-        <v>0</v>
-      </c>
-      <c r="H243" s="32"/>
+      <c r="G243" s="31">
+        <v>0</v>
+      </c>
+      <c r="H243" s="31"/>
       <c r="I243" s="9" t="s">
         <v>725</v>
       </c>
@@ -9894,10 +10022,10 @@
       <c r="F244" s="9" t="s">
         <v>727</v>
       </c>
-      <c r="G244" s="32">
-        <v>0</v>
-      </c>
-      <c r="H244" s="32"/>
+      <c r="G244" s="31">
+        <v>0</v>
+      </c>
+      <c r="H244" s="31"/>
       <c r="I244" s="9" t="s">
         <v>728</v>
       </c>
@@ -9921,10 +10049,10 @@
       <c r="F245" s="9" t="s">
         <v>731</v>
       </c>
-      <c r="G245" s="32">
-        <v>0</v>
-      </c>
-      <c r="H245" s="32"/>
+      <c r="G245" s="31">
+        <v>0</v>
+      </c>
+      <c r="H245" s="31"/>
       <c r="I245" s="9" t="s">
         <v>732</v>
       </c>
@@ -9948,10 +10076,10 @@
       <c r="F246" s="9" t="s">
         <v>734</v>
       </c>
-      <c r="G246" s="32">
-        <v>0</v>
-      </c>
-      <c r="H246" s="32"/>
+      <c r="G246" s="31">
+        <v>0</v>
+      </c>
+      <c r="H246" s="31"/>
       <c r="I246" s="9" t="s">
         <v>735</v>
       </c>
@@ -9975,10 +10103,10 @@
       <c r="F247" s="9" t="s">
         <v>737</v>
       </c>
-      <c r="G247" s="32">
-        <v>0</v>
-      </c>
-      <c r="H247" s="32"/>
+      <c r="G247" s="31">
+        <v>0</v>
+      </c>
+      <c r="H247" s="31"/>
       <c r="I247" s="9" t="s">
         <v>738</v>
       </c>
@@ -10002,10 +10130,10 @@
       <c r="F248" s="9" t="s">
         <v>741</v>
       </c>
-      <c r="G248" s="32">
-        <v>0</v>
-      </c>
-      <c r="H248" s="32"/>
+      <c r="G248" s="31">
+        <v>0</v>
+      </c>
+      <c r="H248" s="31"/>
       <c r="I248" s="9" t="s">
         <v>742</v>
       </c>
@@ -10029,10 +10157,10 @@
       <c r="F249" s="9" t="s">
         <v>744</v>
       </c>
-      <c r="G249" s="32">
-        <v>0</v>
-      </c>
-      <c r="H249" s="32"/>
+      <c r="G249" s="31">
+        <v>0</v>
+      </c>
+      <c r="H249" s="31"/>
       <c r="I249" s="9" t="s">
         <v>745</v>
       </c>
@@ -10056,10 +10184,10 @@
       <c r="F250" s="9" t="s">
         <v>747</v>
       </c>
-      <c r="G250" s="32">
-        <v>0</v>
-      </c>
-      <c r="H250" s="32"/>
+      <c r="G250" s="31">
+        <v>0</v>
+      </c>
+      <c r="H250" s="31"/>
       <c r="I250" s="9" t="s">
         <v>748</v>
       </c>
@@ -10083,10 +10211,10 @@
       <c r="F251" s="9" t="s">
         <v>750</v>
       </c>
-      <c r="G251" s="32">
-        <v>0</v>
-      </c>
-      <c r="H251" s="32"/>
+      <c r="G251" s="31">
+        <v>0</v>
+      </c>
+      <c r="H251" s="31"/>
       <c r="I251" s="9" t="s">
         <v>751</v>
       </c>
@@ -10110,10 +10238,10 @@
       <c r="F252" s="9" t="s">
         <v>753</v>
       </c>
-      <c r="G252" s="32">
-        <v>0</v>
-      </c>
-      <c r="H252" s="32"/>
+      <c r="G252" s="31">
+        <v>0</v>
+      </c>
+      <c r="H252" s="31"/>
       <c r="I252" s="9" t="s">
         <v>754</v>
       </c>
@@ -10137,10 +10265,10 @@
       <c r="F253" s="9" t="s">
         <v>756</v>
       </c>
-      <c r="G253" s="32">
-        <v>0</v>
-      </c>
-      <c r="H253" s="32"/>
+      <c r="G253" s="31">
+        <v>0</v>
+      </c>
+      <c r="H253" s="31"/>
       <c r="I253" s="9" t="s">
         <v>757</v>
       </c>
@@ -10164,10 +10292,10 @@
       <c r="F254" s="9" t="s">
         <v>759</v>
       </c>
-      <c r="G254" s="32">
-        <v>0</v>
-      </c>
-      <c r="H254" s="32"/>
+      <c r="G254" s="31">
+        <v>0</v>
+      </c>
+      <c r="H254" s="31"/>
       <c r="I254" s="9" t="s">
         <v>760</v>
       </c>
@@ -10191,10 +10319,10 @@
       <c r="F255" s="9" t="s">
         <v>762</v>
       </c>
-      <c r="G255" s="32">
-        <v>0</v>
-      </c>
-      <c r="H255" s="32"/>
+      <c r="G255" s="31">
+        <v>0</v>
+      </c>
+      <c r="H255" s="31"/>
       <c r="I255" s="9" t="s">
         <v>763</v>
       </c>
@@ -10218,10 +10346,10 @@
       <c r="F256" s="9" t="s">
         <v>765</v>
       </c>
-      <c r="G256" s="32">
-        <v>0</v>
-      </c>
-      <c r="H256" s="32"/>
+      <c r="G256" s="31">
+        <v>0</v>
+      </c>
+      <c r="H256" s="31"/>
       <c r="I256" s="9" t="s">
         <v>766</v>
       </c>
@@ -10245,10 +10373,10 @@
       <c r="F257" s="9" t="s">
         <v>768</v>
       </c>
-      <c r="G257" s="32">
-        <v>0</v>
-      </c>
-      <c r="H257" s="32"/>
+      <c r="G257" s="31">
+        <v>0</v>
+      </c>
+      <c r="H257" s="31"/>
       <c r="I257" s="9" t="s">
         <v>769</v>
       </c>
@@ -10272,10 +10400,10 @@
       <c r="F258" s="9" t="s">
         <v>771</v>
       </c>
-      <c r="G258" s="32">
-        <v>0</v>
-      </c>
-      <c r="H258" s="32"/>
+      <c r="G258" s="31">
+        <v>0</v>
+      </c>
+      <c r="H258" s="31"/>
       <c r="I258" s="9" t="s">
         <v>772</v>
       </c>
@@ -10299,10 +10427,10 @@
       <c r="F259" s="9" t="s">
         <v>774</v>
       </c>
-      <c r="G259" s="32">
-        <v>0</v>
-      </c>
-      <c r="H259" s="32"/>
+      <c r="G259" s="31">
+        <v>0</v>
+      </c>
+      <c r="H259" s="31"/>
       <c r="I259" s="9" t="s">
         <v>775</v>
       </c>
@@ -10326,10 +10454,10 @@
       <c r="F260" s="9" t="s">
         <v>777</v>
       </c>
-      <c r="G260" s="32">
-        <v>0</v>
-      </c>
-      <c r="H260" s="32"/>
+      <c r="G260" s="31">
+        <v>0</v>
+      </c>
+      <c r="H260" s="31"/>
       <c r="I260" s="9" t="s">
         <v>778</v>
       </c>
@@ -10353,10 +10481,10 @@
       <c r="F261" s="9" t="s">
         <v>780</v>
       </c>
-      <c r="G261" s="32">
-        <v>0</v>
-      </c>
-      <c r="H261" s="32"/>
+      <c r="G261" s="31">
+        <v>0</v>
+      </c>
+      <c r="H261" s="31"/>
       <c r="I261" s="9" t="s">
         <v>781</v>
       </c>
@@ -10380,10 +10508,10 @@
       <c r="F262" s="9" t="s">
         <v>783</v>
       </c>
-      <c r="G262" s="32">
-        <v>0</v>
-      </c>
-      <c r="H262" s="32"/>
+      <c r="G262" s="31">
+        <v>0</v>
+      </c>
+      <c r="H262" s="31"/>
       <c r="I262" s="9" t="s">
         <v>784</v>
       </c>
@@ -10407,10 +10535,10 @@
       <c r="F263" s="9" t="s">
         <v>786</v>
       </c>
-      <c r="G263" s="32">
-        <v>0</v>
-      </c>
-      <c r="H263" s="32"/>
+      <c r="G263" s="31">
+        <v>0</v>
+      </c>
+      <c r="H263" s="31"/>
       <c r="I263" s="9" t="s">
         <v>787</v>
       </c>
@@ -10434,10 +10562,10 @@
       <c r="F264" s="9" t="s">
         <v>789</v>
       </c>
-      <c r="G264" s="32">
-        <v>0</v>
-      </c>
-      <c r="H264" s="32"/>
+      <c r="G264" s="31">
+        <v>0</v>
+      </c>
+      <c r="H264" s="31"/>
       <c r="I264" s="9" t="s">
         <v>790</v>
       </c>
@@ -10461,10 +10589,10 @@
       <c r="F265" s="21" t="s">
         <v>792</v>
       </c>
-      <c r="G265" s="33">
-        <v>0</v>
-      </c>
-      <c r="H265" s="33"/>
+      <c r="G265" s="32">
+        <v>0</v>
+      </c>
+      <c r="H265" s="32"/>
       <c r="I265" s="21" t="s">
         <v>793</v>
       </c>
@@ -10480,10 +10608,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -10530,7 +10658,7 @@
       <c r="A11" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="29" t="s">
         <v>25</v>
       </c>
       <c r="E11" s="16">
@@ -10538,14 +10666,14 @@
       </c>
       <c r="F11">
         <f>COUNTIF(Studies!G:G, E11)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G11" t="s">
         <v>794</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="D12" s="30"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="13">
         <v>2</v>
       </c>
@@ -10558,7 +10686,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="D13" s="30"/>
+      <c r="D13" s="29"/>
       <c r="E13" s="22">
         <v>3</v>
       </c>
@@ -10571,21 +10699,21 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="D14" s="30"/>
+      <c r="D14" s="29"/>
       <c r="E14" s="23">
         <v>4</v>
       </c>
       <c r="F14">
         <f>COUNTIF(Studies!G:G, E14)</f>
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="G14" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="D15" s="30"/>
-      <c r="E15" s="28">
+      <c r="D15" s="29"/>
+      <c r="E15" s="27">
         <v>5</v>
       </c>
       <c r="F15">
@@ -10597,13 +10725,13 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="D16" s="30"/>
-      <c r="E16" s="27">
+      <c r="D16" s="29"/>
+      <c r="E16" s="26">
         <v>6</v>
       </c>
       <c r="F16">
         <f>COUNTIF(Studies!G:G, E16)</f>
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="G16" t="s">
         <v>823</v>
@@ -10625,7 +10753,7 @@
       </c>
     </row>
     <row r="18" spans="4:7">
-      <c r="D18" s="26" t="s">
+      <c r="D18" s="36" t="s">
         <v>807</v>
       </c>
       <c r="E18" s="18">
@@ -10640,7 +10768,7 @@
       </c>
     </row>
     <row r="19" spans="4:7">
-      <c r="D19" s="26"/>
+      <c r="D19" s="36"/>
       <c r="E19" s="19">
         <v>9</v>
       </c>
@@ -10653,114 +10781,143 @@
       </c>
     </row>
     <row r="20" spans="4:7">
-      <c r="D20" s="15" t="s">
-        <v>806</v>
-      </c>
-      <c r="E20" s="12">
-        <v>0</v>
+      <c r="D20" s="35" t="s">
+        <v>848</v>
+      </c>
+      <c r="E20" s="34">
+        <v>-1</v>
       </c>
       <c r="F20">
         <f>COUNTIF(Studies!G:G, E20)</f>
-        <v>180</v>
+        <v>25</v>
       </c>
       <c r="G20" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7">
+      <c r="D21" s="15" t="s">
+        <v>806</v>
+      </c>
+      <c r="E21" s="12">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f>COUNTIF(Studies!G:G, E21)</f>
+        <v>132</v>
+      </c>
+      <c r="G21" t="s">
         <v>805</v>
       </c>
     </row>
-    <row r="22" spans="4:7">
-      <c r="D22" t="s">
+    <row r="23" spans="4:7">
+      <c r="D23" t="s">
         <v>847</v>
       </c>
-      <c r="E22">
-        <f>SUM(F11:F19)</f>
-        <v>84</v>
-      </c>
-      <c r="F22" s="31">
-        <f>E22/E22</f>
+      <c r="E23">
+        <f>SUM(F11:F20)</f>
+        <v>132</v>
+      </c>
+      <c r="F23" s="30">
+        <f>E23/E23</f>
         <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="4:7">
-      <c r="D24" t="s">
-        <v>846</v>
-      </c>
-      <c r="E24">
-        <f>F11+F14</f>
-        <v>44</v>
-      </c>
-      <c r="F24" s="29">
-        <f>E24/E22</f>
-        <v>0.52380952380952384</v>
       </c>
     </row>
     <row r="25" spans="4:7">
       <c r="D25" t="s">
+        <v>846</v>
+      </c>
+      <c r="E25">
+        <f>F11+F14</f>
+        <v>58</v>
+      </c>
+      <c r="F25" s="28">
+        <f>E25/E23</f>
+        <v>0.43939393939393939</v>
+      </c>
+    </row>
+    <row r="26" spans="4:7">
+      <c r="D26" t="s">
         <v>835</v>
       </c>
-      <c r="E25">
+      <c r="E26">
         <f>F13+F15+F17+F18</f>
         <v>16</v>
       </c>
-      <c r="F25" s="29">
-        <f>E25/E22</f>
-        <v>0.19047619047619047</v>
-      </c>
-    </row>
-    <row r="26" spans="4:7">
-      <c r="D26" t="s">
-        <v>845</v>
-      </c>
-      <c r="E26">
-        <f>F16+F19</f>
-        <v>24</v>
-      </c>
-      <c r="F26" s="29">
-        <f>E26/E22</f>
-        <v>0.2857142857142857</v>
+      <c r="F26" s="28">
+        <f>E26/E23</f>
+        <v>0.12121212121212122</v>
       </c>
     </row>
     <row r="27" spans="4:7">
       <c r="D27" t="s">
+        <v>845</v>
+      </c>
+      <c r="E27">
+        <f>F16+F19</f>
+        <v>33</v>
+      </c>
+      <c r="F27" s="28">
+        <f>E27/E23</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="28" spans="4:7">
+      <c r="D28" t="s">
         <v>834</v>
       </c>
-      <c r="E27">
+      <c r="E28">
         <f>F13</f>
         <v>9</v>
       </c>
-      <c r="F27" s="29">
-        <f>F13/E22</f>
-        <v>0.10714285714285714</v>
-      </c>
-    </row>
-    <row r="29" spans="4:7">
-      <c r="D29" t="s">
-        <v>825</v>
-      </c>
-      <c r="E29">
-        <f>SUM(F11:F19)</f>
-        <v>84</v>
-      </c>
-      <c r="F29" s="29">
-        <f>E29/SUM(F11:F20)</f>
-        <v>0.31818181818181818</v>
+      <c r="F28" s="28">
+        <f>F13/E23</f>
+        <v>6.8181818181818177E-2</v>
       </c>
     </row>
     <row r="30" spans="4:7">
       <c r="D30" t="s">
+        <v>825</v>
+      </c>
+      <c r="E30">
+        <f>SUM(F11:F20)</f>
+        <v>132</v>
+      </c>
+      <c r="F30" s="28">
+        <f>E30/SUM(F11:F21)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="4:7">
+      <c r="D31" t="s">
         <v>836</v>
       </c>
-      <c r="E30">
-        <f>F20</f>
-        <v>180</v>
-      </c>
-      <c r="F30" s="29">
-        <f>F20/SUM(F11:F20)</f>
-        <v>0.68181818181818177</v>
+      <c r="E31">
+        <f>F21</f>
+        <v>132</v>
+      </c>
+      <c r="F31" s="28">
+        <f>F21/SUM(F11:F21)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="4:7">
+      <c r="D32" t="s">
+        <v>851</v>
+      </c>
+      <c r="E32">
+        <f>E30+E31</f>
+        <v>264</v>
+      </c>
+      <c r="F32" s="28">
+        <f>E32/E32</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="D11:D16"/>
+    <mergeCell ref="D18:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add more analyzed papers
</commit_message>
<xml_diff>
--- a/literature_search/LoS_incentives_revision_micro.xlsx
+++ b/literature_search/LoS_incentives_revision_micro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petr/code/meta/incentives/literature_search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED45911D-DB93-424C-BC9A-99E63A828322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169DDD65-8F61-5B48-9B93-79F855889B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29400" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Studies" sheetId="13" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1332" uniqueCount="858">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="860">
   <si>
     <t>Journal</t>
   </si>
@@ -2612,6 +2612,12 @@
   </si>
   <si>
     <t>Irrelevant dependent variable (acceptance)</t>
+  </si>
+  <si>
+    <t>New Journal</t>
+  </si>
+  <si>
+    <t>Unavailable</t>
   </si>
 </sst>
 </file>
@@ -3189,10 +3195,10 @@
   </sheetPr>
   <dimension ref="A1:I265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="135" zoomScaleNormal="131" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A189" zoomScale="135" zoomScaleNormal="131" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection activeCell="A117" sqref="A117"/>
-      <selection pane="topRight" activeCell="H154" sqref="H154"/>
+      <selection pane="topRight" activeCell="F196" sqref="F196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7526,7 +7532,7 @@
         <v>5</v>
       </c>
       <c r="H150" s="30" t="s">
-        <v>827</v>
+        <v>858</v>
       </c>
       <c r="I150" s="9" t="s">
         <v>477</v>
@@ -7555,7 +7561,7 @@
         <v>5</v>
       </c>
       <c r="H151" s="30" t="s">
-        <v>827</v>
+        <v>858</v>
       </c>
       <c r="I151" s="9" t="s">
         <v>480</v>
@@ -7584,7 +7590,7 @@
         <v>5</v>
       </c>
       <c r="H152" s="30" t="s">
-        <v>827</v>
+        <v>858</v>
       </c>
       <c r="I152" s="9" t="s">
         <v>483</v>
@@ -7613,7 +7619,7 @@
         <v>5</v>
       </c>
       <c r="H153" s="30" t="s">
-        <v>827</v>
+        <v>858</v>
       </c>
       <c r="I153" s="9" t="s">
         <v>486</v>
@@ -7642,7 +7648,7 @@
         <v>5</v>
       </c>
       <c r="H154" s="30" t="s">
-        <v>827</v>
+        <v>858</v>
       </c>
       <c r="I154" s="9" t="s">
         <v>489</v>
@@ -7668,9 +7674,11 @@
         <v>491</v>
       </c>
       <c r="G155" s="30">
-        <v>0</v>
-      </c>
-      <c r="H155" s="30"/>
+        <v>5</v>
+      </c>
+      <c r="H155" s="30" t="s">
+        <v>858</v>
+      </c>
       <c r="I155" s="9" t="s">
         <v>492</v>
       </c>
@@ -7695,9 +7703,11 @@
         <v>493</v>
       </c>
       <c r="G156" s="30">
-        <v>0</v>
-      </c>
-      <c r="H156" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="H156" s="30" t="s">
+        <v>831</v>
+      </c>
       <c r="I156" s="9" t="s">
         <v>494</v>
       </c>
@@ -7722,9 +7732,11 @@
         <v>496</v>
       </c>
       <c r="G157" s="30">
-        <v>0</v>
-      </c>
-      <c r="H157" s="30"/>
+        <v>5</v>
+      </c>
+      <c r="H157" s="30" t="s">
+        <v>858</v>
+      </c>
       <c r="I157" s="9" t="s">
         <v>497</v>
       </c>
@@ -7749,9 +7761,11 @@
         <v>499</v>
       </c>
       <c r="G158" s="30">
-        <v>0</v>
-      </c>
-      <c r="H158" s="30"/>
+        <v>5</v>
+      </c>
+      <c r="H158" s="30" t="s">
+        <v>858</v>
+      </c>
       <c r="I158" s="9" t="s">
         <v>500</v>
       </c>
@@ -7776,9 +7790,11 @@
         <v>502</v>
       </c>
       <c r="G159" s="30">
-        <v>0</v>
-      </c>
-      <c r="H159" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="H159" s="30" t="s">
+        <v>831</v>
+      </c>
       <c r="I159" s="9" t="s">
         <v>503</v>
       </c>
@@ -7803,9 +7819,11 @@
         <v>505</v>
       </c>
       <c r="G160" s="30">
-        <v>0</v>
-      </c>
-      <c r="H160" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="H160" s="30" t="s">
+        <v>831</v>
+      </c>
       <c r="I160" s="9" t="s">
         <v>506</v>
       </c>
@@ -7830,9 +7848,11 @@
         <v>508</v>
       </c>
       <c r="G161" s="30">
-        <v>0</v>
-      </c>
-      <c r="H161" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="H161" s="30" t="s">
+        <v>859</v>
+      </c>
       <c r="I161" s="9" t="s">
         <v>509</v>
       </c>
@@ -7857,9 +7877,11 @@
         <v>511</v>
       </c>
       <c r="G162" s="30">
-        <v>0</v>
-      </c>
-      <c r="H162" s="30"/>
+        <v>-1</v>
+      </c>
+      <c r="H162" s="30" t="s">
+        <v>836</v>
+      </c>
       <c r="I162" s="9" t="s">
         <v>512</v>
       </c>
@@ -7884,9 +7906,11 @@
         <v>514</v>
       </c>
       <c r="G163" s="30">
-        <v>0</v>
-      </c>
-      <c r="H163" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="H163" s="30" t="s">
+        <v>840</v>
+      </c>
       <c r="I163" s="9" t="s">
         <v>515</v>
       </c>
@@ -7911,9 +7935,11 @@
         <v>505</v>
       </c>
       <c r="G164" s="30">
-        <v>0</v>
-      </c>
-      <c r="H164" s="30"/>
+        <v>-1</v>
+      </c>
+      <c r="H164" s="30" t="s">
+        <v>836</v>
+      </c>
       <c r="I164" s="9" t="s">
         <v>517</v>
       </c>
@@ -7938,9 +7964,11 @@
         <v>519</v>
       </c>
       <c r="G165" s="30">
-        <v>0</v>
-      </c>
-      <c r="H165" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="H165" s="30" t="s">
+        <v>831</v>
+      </c>
       <c r="I165" s="9" t="s">
         <v>520</v>
       </c>
@@ -7965,9 +7993,11 @@
         <v>522</v>
       </c>
       <c r="G166" s="30">
-        <v>0</v>
-      </c>
-      <c r="H166" s="30"/>
+        <v>5</v>
+      </c>
+      <c r="H166" s="30" t="s">
+        <v>858</v>
+      </c>
       <c r="I166" s="9" t="s">
         <v>523</v>
       </c>
@@ -7992,9 +8022,11 @@
         <v>525</v>
       </c>
       <c r="G167" s="30">
-        <v>0</v>
-      </c>
-      <c r="H167" s="30"/>
+        <v>5</v>
+      </c>
+      <c r="H167" s="30" t="s">
+        <v>858</v>
+      </c>
       <c r="I167" s="9" t="s">
         <v>526</v>
       </c>
@@ -8019,9 +8051,11 @@
         <v>528</v>
       </c>
       <c r="G168" s="30">
-        <v>0</v>
-      </c>
-      <c r="H168" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="H168" s="30" t="s">
+        <v>840</v>
+      </c>
       <c r="I168" s="9" t="s">
         <v>529</v>
       </c>
@@ -8046,9 +8080,11 @@
         <v>531</v>
       </c>
       <c r="G169" s="30">
-        <v>0</v>
-      </c>
-      <c r="H169" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="H169" s="30" t="s">
+        <v>831</v>
+      </c>
       <c r="I169" s="9" t="s">
         <v>532</v>
       </c>
@@ -8073,9 +8109,11 @@
         <v>534</v>
       </c>
       <c r="G170" s="30">
-        <v>0</v>
-      </c>
-      <c r="H170" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="H170" s="30" t="s">
+        <v>840</v>
+      </c>
       <c r="I170" s="9" t="s">
         <v>535</v>
       </c>
@@ -8100,9 +8138,11 @@
         <v>537</v>
       </c>
       <c r="G171" s="30">
-        <v>0</v>
-      </c>
-      <c r="H171" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="H171" s="30" t="s">
+        <v>840</v>
+      </c>
       <c r="I171" s="9" t="s">
         <v>538</v>
       </c>
@@ -8127,9 +8167,11 @@
         <v>540</v>
       </c>
       <c r="G172" s="30">
-        <v>0</v>
-      </c>
-      <c r="H172" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="H172" s="30" t="s">
+        <v>831</v>
+      </c>
       <c r="I172" s="9" t="s">
         <v>541</v>
       </c>
@@ -8154,9 +8196,11 @@
         <v>542</v>
       </c>
       <c r="G173" s="30">
-        <v>0</v>
-      </c>
-      <c r="H173" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="H173" s="30" t="s">
+        <v>831</v>
+      </c>
       <c r="I173" s="9" t="s">
         <v>543</v>
       </c>
@@ -8181,9 +8225,11 @@
         <v>545</v>
       </c>
       <c r="G174" s="30">
-        <v>0</v>
-      </c>
-      <c r="H174" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="H174" s="30" t="s">
+        <v>840</v>
+      </c>
       <c r="I174" s="9" t="s">
         <v>546</v>
       </c>
@@ -8208,9 +8254,11 @@
         <v>548</v>
       </c>
       <c r="G175" s="30">
-        <v>0</v>
-      </c>
-      <c r="H175" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="H175" s="30" t="s">
+        <v>840</v>
+      </c>
       <c r="I175" s="9" t="s">
         <v>549</v>
       </c>
@@ -8235,9 +8283,11 @@
         <v>551</v>
       </c>
       <c r="G176" s="30">
-        <v>0</v>
-      </c>
-      <c r="H176" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="H176" s="30" t="s">
+        <v>831</v>
+      </c>
       <c r="I176" s="9" t="s">
         <v>552</v>
       </c>
@@ -8262,9 +8312,11 @@
         <v>554</v>
       </c>
       <c r="G177" s="30">
-        <v>0</v>
-      </c>
-      <c r="H177" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="H177" s="30" t="s">
+        <v>831</v>
+      </c>
       <c r="I177" s="9" t="s">
         <v>555</v>
       </c>
@@ -8289,9 +8341,11 @@
         <v>558</v>
       </c>
       <c r="G178" s="30">
-        <v>0</v>
-      </c>
-      <c r="H178" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="H178" s="30" t="s">
+        <v>840</v>
+      </c>
       <c r="I178" s="9" t="s">
         <v>559</v>
       </c>
@@ -8316,9 +8370,11 @@
         <v>561</v>
       </c>
       <c r="G179" s="30">
-        <v>0</v>
-      </c>
-      <c r="H179" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="H179" s="30" t="s">
+        <v>840</v>
+      </c>
       <c r="I179" s="9" t="s">
         <v>562</v>
       </c>
@@ -8343,9 +8399,11 @@
         <v>564</v>
       </c>
       <c r="G180" s="30">
-        <v>0</v>
-      </c>
-      <c r="H180" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="H180" s="30" t="s">
+        <v>840</v>
+      </c>
       <c r="I180" s="9" t="s">
         <v>565</v>
       </c>
@@ -8370,9 +8428,11 @@
         <v>476</v>
       </c>
       <c r="G181" s="30">
-        <v>0</v>
-      </c>
-      <c r="H181" s="30"/>
+        <v>-1</v>
+      </c>
+      <c r="H181" s="30" t="s">
+        <v>836</v>
+      </c>
       <c r="I181" s="9" t="s">
         <v>567</v>
       </c>
@@ -8397,9 +8457,11 @@
         <v>457</v>
       </c>
       <c r="G182" s="30">
-        <v>0</v>
-      </c>
-      <c r="H182" s="30"/>
+        <v>-1</v>
+      </c>
+      <c r="H182" s="30" t="s">
+        <v>836</v>
+      </c>
       <c r="I182" s="9" t="s">
         <v>458</v>
       </c>
@@ -8424,9 +8486,11 @@
         <v>485</v>
       </c>
       <c r="G183" s="30">
-        <v>0</v>
-      </c>
-      <c r="H183" s="30"/>
+        <v>-1</v>
+      </c>
+      <c r="H183" s="30" t="s">
+        <v>836</v>
+      </c>
       <c r="I183" s="9" t="s">
         <v>486</v>
       </c>
@@ -8451,9 +8515,11 @@
         <v>569</v>
       </c>
       <c r="G184" s="30">
-        <v>0</v>
-      </c>
-      <c r="H184" s="30"/>
+        <v>5</v>
+      </c>
+      <c r="H184" s="30" t="s">
+        <v>858</v>
+      </c>
       <c r="I184" s="9" t="s">
         <v>570</v>
       </c>
@@ -8478,9 +8544,11 @@
         <v>482</v>
       </c>
       <c r="G185" s="30">
-        <v>0</v>
-      </c>
-      <c r="H185" s="30"/>
+        <v>-1</v>
+      </c>
+      <c r="H185" s="30" t="s">
+        <v>836</v>
+      </c>
       <c r="I185" s="9" t="s">
         <v>571</v>
       </c>
@@ -8505,9 +8573,11 @@
         <v>479</v>
       </c>
       <c r="G186" s="30">
-        <v>0</v>
-      </c>
-      <c r="H186" s="30"/>
+        <v>-1</v>
+      </c>
+      <c r="H186" s="30" t="s">
+        <v>836</v>
+      </c>
       <c r="I186" s="9" t="s">
         <v>480</v>
       </c>
@@ -8532,9 +8602,11 @@
         <v>488</v>
       </c>
       <c r="G187" s="30">
-        <v>0</v>
-      </c>
-      <c r="H187" s="30"/>
+        <v>-1</v>
+      </c>
+      <c r="H187" s="30" t="s">
+        <v>836</v>
+      </c>
       <c r="I187" s="9" t="s">
         <v>572</v>
       </c>
@@ -8559,9 +8631,11 @@
         <v>460</v>
       </c>
       <c r="G188" s="30">
-        <v>0</v>
-      </c>
-      <c r="H188" s="30"/>
+        <v>-1</v>
+      </c>
+      <c r="H188" s="30" t="s">
+        <v>836</v>
+      </c>
       <c r="I188" s="9" t="s">
         <v>573</v>
       </c>
@@ -8586,9 +8660,11 @@
         <v>575</v>
       </c>
       <c r="G189" s="30">
-        <v>0</v>
-      </c>
-      <c r="H189" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="H189" s="30" t="s">
+        <v>831</v>
+      </c>
       <c r="I189" s="9" t="s">
         <v>576</v>
       </c>
@@ -8613,9 +8689,11 @@
         <v>578</v>
       </c>
       <c r="G190" s="30">
-        <v>0</v>
-      </c>
-      <c r="H190" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="H190" s="30" t="s">
+        <v>840</v>
+      </c>
       <c r="I190" s="9" t="s">
         <v>579</v>
       </c>
@@ -8640,9 +8718,11 @@
         <v>581</v>
       </c>
       <c r="G191" s="30">
-        <v>0</v>
-      </c>
-      <c r="H191" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="H191" s="30" t="s">
+        <v>831</v>
+      </c>
       <c r="I191" s="9" t="s">
         <v>582</v>
       </c>
@@ -8667,9 +8747,11 @@
         <v>496</v>
       </c>
       <c r="G192" s="30">
-        <v>0</v>
-      </c>
-      <c r="H192" s="30"/>
+        <v>-1</v>
+      </c>
+      <c r="H192" s="30" t="s">
+        <v>836</v>
+      </c>
       <c r="I192" s="9" t="s">
         <v>497</v>
       </c>
@@ -8694,9 +8776,11 @@
         <v>584</v>
       </c>
       <c r="G193" s="30">
-        <v>0</v>
-      </c>
-      <c r="H193" s="30"/>
+        <v>5</v>
+      </c>
+      <c r="H193" s="30" t="s">
+        <v>858</v>
+      </c>
       <c r="I193" s="9" t="s">
         <v>585</v>
       </c>
@@ -8721,9 +8805,11 @@
         <v>463</v>
       </c>
       <c r="G194" s="30">
-        <v>0</v>
-      </c>
-      <c r="H194" s="30"/>
+        <v>-1</v>
+      </c>
+      <c r="H194" s="30" t="s">
+        <v>836</v>
+      </c>
       <c r="I194" s="9" t="s">
         <v>586</v>
       </c>
@@ -8748,9 +8834,11 @@
         <v>493</v>
       </c>
       <c r="G195" s="30">
-        <v>0</v>
-      </c>
-      <c r="H195" s="30"/>
+        <v>-1</v>
+      </c>
+      <c r="H195" s="30" t="s">
+        <v>836</v>
+      </c>
       <c r="I195" s="9" t="s">
         <v>587</v>
       </c>
@@ -10846,7 +10934,7 @@
       </c>
       <c r="F15">
         <f>COUNTIF(Studies!G:G, E15)</f>
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="G15" t="s">
         <v>821</v>
@@ -10859,7 +10947,7 @@
       </c>
       <c r="F16">
         <f>COUNTIF(Studies!G:G, E16)</f>
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="G16" t="s">
         <v>822</v>
@@ -10917,7 +11005,7 @@
       </c>
       <c r="F20">
         <f>COUNTIF(Studies!G:G, E20)</f>
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="G20" t="s">
         <v>848</v>
@@ -10932,7 +11020,7 @@
       </c>
       <c r="F21">
         <f>COUNTIF(Studies!G:G, E21)</f>
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="G21" t="s">
         <v>804</v>
@@ -10944,7 +11032,7 @@
       </c>
       <c r="E23">
         <f>SUM(F11:F20)</f>
-        <v>201</v>
+        <v>242</v>
       </c>
       <c r="F23" s="29">
         <f>E23/E23</f>
@@ -10961,7 +11049,7 @@
       </c>
       <c r="F25" s="28">
         <f>E25/E23</f>
-        <v>0.43283582089552236</v>
+        <v>0.35950413223140498</v>
       </c>
     </row>
     <row r="26" spans="4:7">
@@ -10970,11 +11058,11 @@
       </c>
       <c r="E26">
         <f>F13+F15+F17+F18</f>
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F26" s="28">
         <f>E26/E23</f>
-        <v>0.1691542288557214</v>
+        <v>0.16942148760330578</v>
       </c>
     </row>
     <row r="27" spans="4:7">
@@ -10983,11 +11071,11 @@
       </c>
       <c r="E27">
         <f>F16+F19</f>
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="F27" s="28">
         <f>E27/E23</f>
-        <v>0.26368159203980102</v>
+        <v>0.30991735537190085</v>
       </c>
     </row>
     <row r="28" spans="4:7">
@@ -11000,7 +11088,7 @@
       </c>
       <c r="F28" s="28">
         <f>F13/E23</f>
-        <v>4.4776119402985072E-2</v>
+        <v>3.71900826446281E-2</v>
       </c>
     </row>
     <row r="30" spans="4:7">
@@ -11009,11 +11097,11 @@
       </c>
       <c r="E30">
         <f>SUM(F11:F20)</f>
-        <v>201</v>
+        <v>242</v>
       </c>
       <c r="F30" s="28">
         <f>E30/SUM(F11:F21)</f>
-        <v>0.76136363636363635</v>
+        <v>0.91666666666666663</v>
       </c>
     </row>
     <row r="31" spans="4:7">
@@ -11022,11 +11110,11 @@
       </c>
       <c r="E31">
         <f>F21</f>
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="F31" s="28">
         <f>F21/SUM(F11:F21)</f>
-        <v>0.23863636363636365</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="32" spans="4:7">

</xml_diff>